<commit_message>
changed the right_arm.ini and left_arm.ini
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/leftArm_ini_generator new.xlsx
+++ b/app/skinGui/iniGenerators/leftArm_ini_generator new.xlsx
@@ -13335,7 +13335,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13423,18 +13423,18 @@
       </c>
       <c r="D3" s="23">
         <f t="shared" ref="D3:D4" si="2">((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
-        <v>136.60254037844388</v>
+        <v>213.39745962155612</v>
       </c>
       <c r="E3" s="23">
-        <f t="shared" ref="E3:E4" si="3">IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
-        <v>-89.999719388456853</v>
+        <f>IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)-$N$5)</f>
+        <v>149.99971938845687</v>
       </c>
       <c r="F3" s="11">
         <v>5</v>
       </c>
       <c r="G3" s="25">
-        <f t="shared" ref="G3:G4" si="4">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G3:G4" si="3">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -13484,18 +13484,18 @@
       </c>
       <c r="D4" s="23">
         <f t="shared" si="2"/>
-        <v>152.60254037844385</v>
+        <v>197.39745962155615</v>
       </c>
       <c r="E4" s="23">
-        <f t="shared" si="3"/>
-        <v>-29.999859694228427</v>
+        <f t="shared" ref="E4:E25" si="4">IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)-$N$5)</f>
+        <v>89.999859694228434</v>
       </c>
       <c r="F4" s="11">
         <v>5</v>
       </c>
       <c r="G4" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -13524,7 +13524,7 @@
         <v>17</v>
       </c>
       <c r="R4" s="57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S4" s="9"/>
     </row>
@@ -13694,7 +13694,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>0</v>
+        <v>-350</v>
       </c>
       <c r="O9" s="45">
         <v>164</v>
@@ -13749,18 +13749,18 @@
       </c>
       <c r="D11" s="23">
         <f t="shared" ref="D11:D12" si="7">((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
-        <v>168.60254037844382</v>
+        <v>181.39745962155618</v>
       </c>
       <c r="E11" s="23">
-        <f t="shared" ref="E11:E12" si="8">IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
       </c>
       <c r="G11" s="25">
-        <f t="shared" ref="G11:G12" si="9">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G11:G12" si="8">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="42">
@@ -13799,18 +13799,18 @@
       </c>
       <c r="D12" s="23">
         <f t="shared" si="7"/>
-        <v>184.60254037844379</v>
+        <v>165.39745962155621</v>
       </c>
       <c r="E12" s="23">
-        <f t="shared" si="8"/>
-        <v>-29.999859694228427</v>
+        <f t="shared" si="4"/>
+        <v>89.999859694228434</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
       <c r="G12" s="25">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="42">
@@ -13838,27 +13838,27 @@
         <v>27</v>
       </c>
       <c r="B13" s="23">
-        <f t="shared" ref="B11:B15" si="10">((ROUND($L13/10,0))-1)*4+MOD($L13,10)+((J13-1)*16)</f>
+        <f t="shared" ref="B13:B15" si="9">((ROUND($L13/10,0))-1)*4+MOD($L13,10)+((J13-1)*16)</f>
         <v>24</v>
       </c>
       <c r="C13" s="23">
-        <f t="shared" ref="C11:C15" si="11">((+O13*COS($N$3)-P13*SIN($N$3)+$N$7)*$R$3)</f>
+        <f t="shared" ref="C13:C15" si="10">((+O13*COS($N$3)-P13*SIN($N$3)+$N$7)*$R$3)</f>
         <v>86.602540378443919</v>
       </c>
       <c r="D13" s="23">
-        <f t="shared" ref="D11:D15" si="12">((O13*SIN($N$3)+P13*COS($N$3)+$N$9)*$R$4)</f>
-        <v>200.60254037844379</v>
+        <f t="shared" ref="D13:D15" si="11">((O13*SIN($N$3)+P13*COS($N$3)+$N$9)*$R$4)</f>
+        <v>149.39745962155621</v>
       </c>
       <c r="E13" s="23">
-        <f t="shared" ref="E11:E15" si="13">IF(($R$3*$R$4)=1,1,-1)*(($M13/3.1416*180)+$N$5)</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
       </c>
       <c r="G13" s="25">
-        <f t="shared" ref="G11:G15" si="14">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G13:G15" si="12">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="42">
@@ -13886,27 +13886,27 @@
         <v>27</v>
       </c>
       <c r="B14" s="23">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="C14" s="23">
         <f t="shared" si="10"/>
-        <v>25</v>
-      </c>
-      <c r="C14" s="23">
+        <v>68.12733176437591</v>
+      </c>
+      <c r="D14" s="23">
         <f t="shared" si="11"/>
-        <v>68.12733176437591</v>
-      </c>
-      <c r="D14" s="23">
-        <f t="shared" si="12"/>
-        <v>200.60254037844379</v>
+        <v>149.39745962155621</v>
       </c>
       <c r="E14" s="23">
-        <f t="shared" si="13"/>
-        <v>89.999859694228434</v>
+        <f t="shared" si="4"/>
+        <v>-29.999859694228427</v>
       </c>
       <c r="F14" s="11">
         <v>5</v>
       </c>
       <c r="G14" s="25">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="42">
@@ -13934,27 +13934,27 @@
         <v>27</v>
       </c>
       <c r="B15" s="23">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="C15" s="23">
         <f t="shared" si="10"/>
-        <v>22</v>
-      </c>
-      <c r="C15" s="23">
+        <v>58.889727457341905</v>
+      </c>
+      <c r="D15" s="23">
         <f t="shared" si="11"/>
-        <v>58.889727457341905</v>
-      </c>
-      <c r="D15" s="23">
-        <f t="shared" si="12"/>
-        <v>216.60254037844379</v>
+        <v>133.39745962155621</v>
       </c>
       <c r="E15" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F15" s="11">
         <v>5</v>
       </c>
       <c r="G15" s="25">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="42">
@@ -14069,27 +14069,27 @@
         <v>27</v>
       </c>
       <c r="B19" s="23">
-        <f t="shared" ref="B19" si="15">((ROUND($L19/10,0))-1)*4+MOD($L19,10)+((J19-1)*16)</f>
+        <f t="shared" ref="B19" si="13">((ROUND($L19/10,0))-1)*4+MOD($L19,10)+((J19-1)*16)</f>
         <v>26</v>
       </c>
       <c r="C19" s="23">
-        <f t="shared" ref="C19" si="16">((+O19*COS($N$3)-P19*SIN($N$3)+$N$7)*$R$3)</f>
+        <f t="shared" ref="C19" si="14">((+O19*COS($N$3)-P19*SIN($N$3)+$N$7)*$R$3)</f>
         <v>58.889727457341891</v>
       </c>
       <c r="D19" s="23">
-        <f t="shared" ref="D19" si="17">((O19*SIN($N$3)+P19*COS($N$3)+$N$9)*$R$4)</f>
-        <v>184.60254037844382</v>
+        <f t="shared" ref="D19" si="15">((O19*SIN($N$3)+P19*COS($N$3)+$N$9)*$R$4)</f>
+        <v>165.39745962155618</v>
       </c>
       <c r="E19" s="23">
-        <f t="shared" ref="E19" si="18">IF(($R$3*$R$4)=1,1,-1)*(($M19/3.1416*180)+$N$5)</f>
-        <v>149.99971938845687</v>
+        <f t="shared" si="4"/>
+        <v>-89.999719388456853</v>
       </c>
       <c r="F19" s="11">
         <v>5</v>
       </c>
       <c r="G19" s="25">
-        <f t="shared" ref="G19" si="19">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G19" si="16">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="42">
@@ -14204,27 +14204,27 @@
         <v>27</v>
       </c>
       <c r="B23" s="23">
-        <f t="shared" ref="B23:B25" si="20">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
+        <f t="shared" ref="B23:B25" si="17">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
         <v>27</v>
       </c>
       <c r="C23" s="23">
-        <f t="shared" ref="C23:C25" si="21">((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
+        <f t="shared" ref="C23:C25" si="18">((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
         <v>68.127331764375896</v>
       </c>
       <c r="D23" s="23">
-        <f t="shared" ref="D23:D25" si="22">((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
-        <v>168.60254037844382</v>
+        <f t="shared" ref="D23:D25" si="19">((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
+        <v>181.39745962155618</v>
       </c>
       <c r="E23" s="23">
-        <f t="shared" ref="E23:E25" si="23">IF(($R$3*$R$4)=1,1,-1)*(($M23/3.1416*180)+$N$5)</f>
-        <v>209.99957908268468</v>
+        <f t="shared" si="4"/>
+        <v>-149.99957908268468</v>
       </c>
       <c r="F23" s="11">
         <v>5</v>
       </c>
       <c r="G23" s="25">
-        <f t="shared" ref="G23:G25" si="24">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G23:G25" si="20">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="42">
@@ -14252,27 +14252,27 @@
         <v>27</v>
       </c>
       <c r="B24" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>30</v>
       </c>
       <c r="C24" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>58.889727457341856</v>
       </c>
       <c r="D24" s="23">
-        <f t="shared" si="22"/>
-        <v>152.60254037844382</v>
+        <f t="shared" si="19"/>
+        <v>197.39745962155618</v>
       </c>
       <c r="E24" s="23">
-        <f t="shared" si="23"/>
-        <v>149.99971938845687</v>
+        <f t="shared" si="4"/>
+        <v>-89.999719388456853</v>
       </c>
       <c r="F24" s="11">
         <v>5</v>
       </c>
       <c r="G24" s="25">
-        <f t="shared" si="24"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>1</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="42">
@@ -14300,27 +14300,27 @@
         <v>27</v>
       </c>
       <c r="B25" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>31</v>
       </c>
       <c r="C25" s="23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>68.127331764375853</v>
       </c>
       <c r="D25" s="23">
-        <f t="shared" si="22"/>
-        <v>136.60254037844385</v>
+        <f t="shared" si="19"/>
+        <v>213.39745962155615</v>
       </c>
       <c r="E25" s="23">
-        <f t="shared" si="23"/>
-        <v>209.99957908268468</v>
+        <f t="shared" si="4"/>
+        <v>-149.99957908268468</v>
       </c>
       <c r="F25" s="11">
         <v>5</v>
       </c>
       <c r="G25" s="25">
-        <f t="shared" si="24"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>1</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="42">
@@ -14363,7 +14363,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G13"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14450,18 +14450,18 @@
       </c>
       <c r="D3" s="23">
         <f t="shared" ref="D3:D13" si="2">((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
-        <v>213.39745962155612</v>
+        <v>136.60254037844388</v>
       </c>
       <c r="E3" s="23">
-        <f t="shared" ref="E3:E13" si="3">IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
-        <v>90.000280611543147</v>
+        <f>IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)-$N$5)</f>
+        <v>329.99971938845687</v>
       </c>
       <c r="F3" s="11">
         <v>5</v>
       </c>
       <c r="G3" s="25">
-        <f t="shared" ref="G3:G13" si="4">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G3:G13" si="3">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -14511,18 +14511,18 @@
       </c>
       <c r="D4" s="23">
         <f t="shared" si="2"/>
-        <v>197.39745962155615</v>
+        <v>152.60254037844385</v>
       </c>
       <c r="E4" s="23">
-        <f t="shared" si="3"/>
-        <v>150.00014030577157</v>
+        <f t="shared" ref="E4:E13" si="4">IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)-$N$5)</f>
+        <v>269.99985969422841</v>
       </c>
       <c r="F4" s="11">
         <v>5</v>
       </c>
       <c r="G4" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -14551,7 +14551,7 @@
         <v>17</v>
       </c>
       <c r="R4" s="57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S4" s="9"/>
     </row>
@@ -14569,18 +14569,18 @@
       </c>
       <c r="D5" s="23">
         <f t="shared" si="2"/>
-        <v>197.39745962155612</v>
+        <v>152.60254037844388</v>
       </c>
       <c r="E5" s="23">
-        <f t="shared" si="3"/>
-        <v>90.000280611543147</v>
+        <f t="shared" si="4"/>
+        <v>329.99971938845687</v>
       </c>
       <c r="F5" s="11">
         <v>5</v>
       </c>
       <c r="G5" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -14626,18 +14626,18 @@
       </c>
       <c r="D6" s="23">
         <f t="shared" si="2"/>
-        <v>181.39745962155615</v>
+        <v>168.60254037844385</v>
       </c>
       <c r="E6" s="23">
-        <f t="shared" si="3"/>
-        <v>150.00014030577157</v>
+        <f t="shared" si="4"/>
+        <v>269.99985969422841</v>
       </c>
       <c r="F6" s="11">
         <v>5</v>
       </c>
       <c r="G6" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -14681,18 +14681,18 @@
       </c>
       <c r="D7" s="23">
         <f t="shared" si="2"/>
-        <v>165.39745962155615</v>
+        <v>184.60254037844385</v>
       </c>
       <c r="E7" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="F7" s="11">
         <v>5</v>
       </c>
       <c r="G7" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -14735,18 +14735,18 @@
       </c>
       <c r="D8" s="23">
         <f t="shared" si="2"/>
-        <v>149.39745962155618</v>
+        <v>200.60254037844382</v>
       </c>
       <c r="E8" s="23">
-        <f t="shared" si="3"/>
-        <v>150.00014030577157</v>
+        <f t="shared" si="4"/>
+        <v>269.99985969422841</v>
       </c>
       <c r="F8" s="11">
         <v>5</v>
       </c>
       <c r="G8" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -14789,18 +14789,18 @@
       </c>
       <c r="D9" s="23">
         <f t="shared" si="2"/>
-        <v>133.39745962155621</v>
+        <v>216.60254037844379</v>
       </c>
       <c r="E9" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="F9" s="11">
         <v>5</v>
       </c>
       <c r="G9" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="42">
@@ -14816,7 +14816,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="O9" s="45">
         <v>164</v>
@@ -14840,18 +14840,18 @@
       </c>
       <c r="D10" s="23">
         <f t="shared" si="2"/>
-        <v>133.39745962155621</v>
+        <v>216.60254037844379</v>
       </c>
       <c r="E10" s="23">
-        <f t="shared" si="3"/>
-        <v>269.99985969422841</v>
+        <f t="shared" si="4"/>
+        <v>150.00014030577157</v>
       </c>
       <c r="F10" s="11">
         <v>5</v>
       </c>
       <c r="G10" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="42">
@@ -14890,18 +14890,18 @@
       </c>
       <c r="D11" s="23">
         <f t="shared" si="2"/>
-        <v>181.39745962155615</v>
+        <v>168.60254037844385</v>
       </c>
       <c r="E11" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
       </c>
       <c r="G11" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="42">
@@ -14941,18 +14941,18 @@
       </c>
       <c r="D12" s="23">
         <f t="shared" si="2"/>
-        <v>165.39745962155618</v>
+        <v>184.60254037844382</v>
       </c>
       <c r="E12" s="23">
-        <f t="shared" si="3"/>
-        <v>150.00014030577157</v>
+        <f t="shared" si="4"/>
+        <v>269.99985969422841</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
       <c r="G12" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="42">
@@ -14989,18 +14989,18 @@
       </c>
       <c r="D13" s="23">
         <f t="shared" si="2"/>
-        <v>149.39745962155621</v>
+        <v>200.60254037844379</v>
       </c>
       <c r="E13" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
       </c>
       <c r="G13" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="42">
@@ -16353,7 +16353,7 @@
   <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G94" sqref="A3:G94"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16389,2761 +16389,2761 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="str">
-        <f>IF(lower!A3=0, "", lower!A3)</f>
-        <v/>
-      </c>
-      <c r="B3" s="63" t="str">
-        <f>IF(lower!B3=0, "", lower!B3)</f>
+        <f>IF(lower!A3="", "", lower!A3)</f>
+        <v/>
+      </c>
+      <c r="B3" s="69" t="str">
+        <f>IF(lower!B3="", "", lower!B3)</f>
         <v/>
       </c>
       <c r="C3" s="69" t="str">
-        <f>IF(lower!C3=0, "", lower!C3)</f>
+        <f>IF(lower!C3="", "", lower!C3)</f>
         <v/>
       </c>
       <c r="D3" s="69" t="str">
-        <f>IF(lower!D3=0, "", lower!D3)</f>
+        <f>IF(lower!D3="", "", lower!D3)</f>
         <v/>
       </c>
       <c r="E3" s="69" t="str">
-        <f>IF(lower!E3=0, "", lower!E3)</f>
-        <v/>
-      </c>
-      <c r="F3" s="63" t="str">
-        <f>IF(lower!F3=0, "", lower!F3)</f>
-        <v/>
-      </c>
-      <c r="G3" s="63" t="str">
-        <f>IF(lower!$A3=0, "", lower!G3)</f>
+        <f>IF(lower!E3="", "", lower!E3)</f>
+        <v/>
+      </c>
+      <c r="F3" s="69" t="str">
+        <f>IF(lower!F3="", "", lower!F3)</f>
+        <v/>
+      </c>
+      <c r="G3" s="69" t="str">
+        <f>IF(lower!G3="", "", lower!G3)</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="str">
-        <f>IF(lower!A4=0, "", lower!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="63" t="str">
-        <f>IF(lower!B4=0, "", lower!B4)</f>
+        <f>IF(lower!A4="", "", lower!A4)</f>
+        <v/>
+      </c>
+      <c r="B4" s="69" t="str">
+        <f>IF(lower!B4="", "", lower!B4)</f>
         <v/>
       </c>
       <c r="C4" s="69" t="str">
-        <f>IF(lower!C4=0, "", lower!C4)</f>
+        <f>IF(lower!C4="", "", lower!C4)</f>
         <v/>
       </c>
       <c r="D4" s="69" t="str">
-        <f>IF(lower!D4=0, "", lower!D4)</f>
+        <f>IF(lower!D4="", "", lower!D4)</f>
         <v/>
       </c>
       <c r="E4" s="69" t="str">
-        <f>IF(lower!E4=0, "", lower!E4)</f>
-        <v/>
-      </c>
-      <c r="F4" s="63" t="str">
-        <f>IF(lower!F4=0, "", lower!F4)</f>
-        <v/>
-      </c>
-      <c r="G4" s="63" t="str">
-        <f>IF(lower!$A4=0, "", lower!G4)</f>
+        <f>IF(lower!E4="", "", lower!E4)</f>
+        <v/>
+      </c>
+      <c r="F4" s="69" t="str">
+        <f>IF(lower!F4="", "", lower!F4)</f>
+        <v/>
+      </c>
+      <c r="G4" s="69" t="str">
+        <f>IF(lower!G4="", "", lower!G4)</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="str">
-        <f>IF(lower!A5=0, "", lower!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="63" t="str">
-        <f>IF(lower!B5=0, "", lower!B5)</f>
+        <f>IF(lower!A5="", "", lower!A5)</f>
+        <v/>
+      </c>
+      <c r="B5" s="69" t="str">
+        <f>IF(lower!B5="", "", lower!B5)</f>
         <v/>
       </c>
       <c r="C5" s="69" t="str">
-        <f>IF(lower!C5=0, "", lower!C5)</f>
+        <f>IF(lower!C5="", "", lower!C5)</f>
         <v/>
       </c>
       <c r="D5" s="69" t="str">
-        <f>IF(lower!D5=0, "", lower!D5)</f>
+        <f>IF(lower!D5="", "", lower!D5)</f>
         <v/>
       </c>
       <c r="E5" s="69" t="str">
-        <f>IF(lower!E5=0, "", lower!E5)</f>
-        <v/>
-      </c>
-      <c r="F5" s="63" t="str">
-        <f>IF(lower!F5=0, "", lower!F5)</f>
-        <v/>
-      </c>
-      <c r="G5" s="63" t="str">
-        <f>IF(lower!$A5=0, "", lower!G5)</f>
+        <f>IF(lower!E5="", "", lower!E5)</f>
+        <v/>
+      </c>
+      <c r="F5" s="69" t="str">
+        <f>IF(lower!F5="", "", lower!F5)</f>
+        <v/>
+      </c>
+      <c r="G5" s="69" t="str">
+        <f>IF(lower!G5="", "", lower!G5)</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="str">
-        <f>IF(lower!A6=0, "", lower!A6)</f>
-        <v/>
-      </c>
-      <c r="B6" s="63" t="str">
-        <f>IF(lower!B6=0, "", lower!B6)</f>
+        <f>IF(lower!A6="", "", lower!A6)</f>
+        <v/>
+      </c>
+      <c r="B6" s="69" t="str">
+        <f>IF(lower!B6="", "", lower!B6)</f>
         <v/>
       </c>
       <c r="C6" s="69" t="str">
-        <f>IF(lower!C6=0, "", lower!C6)</f>
+        <f>IF(lower!C6="", "", lower!C6)</f>
         <v/>
       </c>
       <c r="D6" s="69" t="str">
-        <f>IF(lower!D6=0, "", lower!D6)</f>
+        <f>IF(lower!D6="", "", lower!D6)</f>
         <v/>
       </c>
       <c r="E6" s="69" t="str">
-        <f>IF(lower!E6=0, "", lower!E6)</f>
-        <v/>
-      </c>
-      <c r="F6" s="63" t="str">
-        <f>IF(lower!F6=0, "", lower!F6)</f>
-        <v/>
-      </c>
-      <c r="G6" s="63" t="str">
-        <f>IF(lower!$A6=0, "", lower!G6)</f>
+        <f>IF(lower!E6="", "", lower!E6)</f>
+        <v/>
+      </c>
+      <c r="F6" s="69" t="str">
+        <f>IF(lower!F6="", "", lower!F6)</f>
+        <v/>
+      </c>
+      <c r="G6" s="69" t="str">
+        <f>IF(lower!G6="", "", lower!G6)</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="str">
-        <f>IF(lower!A7=0, "", lower!A7)</f>
-        <v/>
-      </c>
-      <c r="B7" s="63" t="str">
-        <f>IF(lower!B7=0, "", lower!B7)</f>
+        <f>IF(lower!A7="", "", lower!A7)</f>
+        <v/>
+      </c>
+      <c r="B7" s="69" t="str">
+        <f>IF(lower!B7="", "", lower!B7)</f>
         <v/>
       </c>
       <c r="C7" s="69" t="str">
-        <f>IF(lower!C7=0, "", lower!C7)</f>
+        <f>IF(lower!C7="", "", lower!C7)</f>
         <v/>
       </c>
       <c r="D7" s="69" t="str">
-        <f>IF(lower!D7=0, "", lower!D7)</f>
+        <f>IF(lower!D7="", "", lower!D7)</f>
         <v/>
       </c>
       <c r="E7" s="69" t="str">
-        <f>IF(lower!E7=0, "", lower!E7)</f>
-        <v/>
-      </c>
-      <c r="F7" s="63" t="str">
-        <f>IF(lower!F7=0, "", lower!F7)</f>
-        <v/>
-      </c>
-      <c r="G7" s="63" t="str">
-        <f>IF(lower!$A7=0, "", lower!G7)</f>
+        <f>IF(lower!E7="", "", lower!E7)</f>
+        <v/>
+      </c>
+      <c r="F7" s="69" t="str">
+        <f>IF(lower!F7="", "", lower!F7)</f>
+        <v/>
+      </c>
+      <c r="G7" s="69" t="str">
+        <f>IF(lower!G7="", "", lower!G7)</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="str">
-        <f>IF(lower!A8=0, "", lower!A8)</f>
-        <v/>
-      </c>
-      <c r="B8" s="63" t="str">
-        <f>IF(lower!B8=0, "", lower!B8)</f>
+        <f>IF(lower!A8="", "", lower!A8)</f>
+        <v/>
+      </c>
+      <c r="B8" s="69" t="str">
+        <f>IF(lower!B8="", "", lower!B8)</f>
         <v/>
       </c>
       <c r="C8" s="69" t="str">
-        <f>IF(lower!C8=0, "", lower!C8)</f>
+        <f>IF(lower!C8="", "", lower!C8)</f>
         <v/>
       </c>
       <c r="D8" s="69" t="str">
-        <f>IF(lower!D8=0, "", lower!D8)</f>
+        <f>IF(lower!D8="", "", lower!D8)</f>
         <v/>
       </c>
       <c r="E8" s="69" t="str">
-        <f>IF(lower!E8=0, "", lower!E8)</f>
-        <v/>
-      </c>
-      <c r="F8" s="63" t="str">
-        <f>IF(lower!F8=0, "", lower!F8)</f>
-        <v/>
-      </c>
-      <c r="G8" s="63" t="str">
-        <f>IF(lower!$A8=0, "", lower!G8)</f>
+        <f>IF(lower!E8="", "", lower!E8)</f>
+        <v/>
+      </c>
+      <c r="F8" s="69" t="str">
+        <f>IF(lower!F8="", "", lower!F8)</f>
+        <v/>
+      </c>
+      <c r="G8" s="69" t="str">
+        <f>IF(lower!G8="", "", lower!G8)</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="str">
-        <f>IF(lower!A9=0, "", lower!A9)</f>
-        <v/>
-      </c>
-      <c r="B9" s="63" t="str">
-        <f>IF(lower!B9=0, "", lower!B9)</f>
+        <f>IF(lower!A9="", "", lower!A9)</f>
+        <v/>
+      </c>
+      <c r="B9" s="69" t="str">
+        <f>IF(lower!B9="", "", lower!B9)</f>
         <v/>
       </c>
       <c r="C9" s="69" t="str">
-        <f>IF(lower!C9=0, "", lower!C9)</f>
+        <f>IF(lower!C9="", "", lower!C9)</f>
         <v/>
       </c>
       <c r="D9" s="69" t="str">
-        <f>IF(lower!D9=0, "", lower!D9)</f>
+        <f>IF(lower!D9="", "", lower!D9)</f>
         <v/>
       </c>
       <c r="E9" s="69" t="str">
-        <f>IF(lower!E9=0, "", lower!E9)</f>
-        <v/>
-      </c>
-      <c r="F9" s="63" t="str">
-        <f>IF(lower!F9=0, "", lower!F9)</f>
-        <v/>
-      </c>
-      <c r="G9" s="63" t="str">
-        <f>IF(lower!$A9=0, "", lower!G9)</f>
+        <f>IF(lower!E9="", "", lower!E9)</f>
+        <v/>
+      </c>
+      <c r="F9" s="69" t="str">
+        <f>IF(lower!F9="", "", lower!F9)</f>
+        <v/>
+      </c>
+      <c r="G9" s="69" t="str">
+        <f>IF(lower!G9="", "", lower!G9)</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="str">
-        <f>IF(lower!A10=0, "", lower!A10)</f>
-        <v/>
-      </c>
-      <c r="B10" s="63" t="str">
-        <f>IF(lower!B10=0, "", lower!B10)</f>
+        <f>IF(lower!A10="", "", lower!A10)</f>
+        <v/>
+      </c>
+      <c r="B10" s="69" t="str">
+        <f>IF(lower!B10="", "", lower!B10)</f>
         <v/>
       </c>
       <c r="C10" s="69" t="str">
-        <f>IF(lower!C10=0, "", lower!C10)</f>
+        <f>IF(lower!C10="", "", lower!C10)</f>
         <v/>
       </c>
       <c r="D10" s="69" t="str">
-        <f>IF(lower!D10=0, "", lower!D10)</f>
+        <f>IF(lower!D10="", "", lower!D10)</f>
         <v/>
       </c>
       <c r="E10" s="69" t="str">
-        <f>IF(lower!E10=0, "", lower!E10)</f>
-        <v/>
-      </c>
-      <c r="F10" s="63" t="str">
-        <f>IF(lower!F10=0, "", lower!F10)</f>
-        <v/>
-      </c>
-      <c r="G10" s="63" t="str">
-        <f>IF(lower!$A10=0, "", lower!G10)</f>
+        <f>IF(lower!E10="", "", lower!E10)</f>
+        <v/>
+      </c>
+      <c r="F10" s="69" t="str">
+        <f>IF(lower!F10="", "", lower!F10)</f>
+        <v/>
+      </c>
+      <c r="G10" s="69" t="str">
+        <f>IF(lower!G10="", "", lower!G10)</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="str">
-        <f>IF(lower!A11=0, "", lower!A11)</f>
-        <v/>
-      </c>
-      <c r="B11" s="63" t="str">
-        <f>IF(lower!B11=0, "", lower!B11)</f>
+        <f>IF(lower!A11="", "", lower!A11)</f>
+        <v/>
+      </c>
+      <c r="B11" s="69" t="str">
+        <f>IF(lower!B11="", "", lower!B11)</f>
         <v/>
       </c>
       <c r="C11" s="69" t="str">
-        <f>IF(lower!C11=0, "", lower!C11)</f>
+        <f>IF(lower!C11="", "", lower!C11)</f>
         <v/>
       </c>
       <c r="D11" s="69" t="str">
-        <f>IF(lower!D11=0, "", lower!D11)</f>
+        <f>IF(lower!D11="", "", lower!D11)</f>
         <v/>
       </c>
       <c r="E11" s="69" t="str">
-        <f>IF(lower!E11=0, "", lower!E11)</f>
-        <v/>
-      </c>
-      <c r="F11" s="63" t="str">
-        <f>IF(lower!F11=0, "", lower!F11)</f>
-        <v/>
-      </c>
-      <c r="G11" s="63" t="str">
-        <f>IF(lower!$A11=0, "", lower!G11)</f>
+        <f>IF(lower!E11="", "", lower!E11)</f>
+        <v/>
+      </c>
+      <c r="F11" s="69" t="str">
+        <f>IF(lower!F11="", "", lower!F11)</f>
+        <v/>
+      </c>
+      <c r="G11" s="69" t="str">
+        <f>IF(lower!G11="", "", lower!G11)</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="str">
-        <f>IF(lower!A12=0, "", lower!A12)</f>
-        <v/>
-      </c>
-      <c r="B12" s="63" t="str">
-        <f>IF(lower!B12=0, "", lower!B12)</f>
+        <f>IF(lower!A12="", "", lower!A12)</f>
+        <v/>
+      </c>
+      <c r="B12" s="69" t="str">
+        <f>IF(lower!B12="", "", lower!B12)</f>
         <v/>
       </c>
       <c r="C12" s="69" t="str">
-        <f>IF(lower!C12=0, "", lower!C12)</f>
+        <f>IF(lower!C12="", "", lower!C12)</f>
         <v/>
       </c>
       <c r="D12" s="69" t="str">
-        <f>IF(lower!D12=0, "", lower!D12)</f>
+        <f>IF(lower!D12="", "", lower!D12)</f>
         <v/>
       </c>
       <c r="E12" s="69" t="str">
-        <f>IF(lower!E12=0, "", lower!E12)</f>
-        <v/>
-      </c>
-      <c r="F12" s="63" t="str">
-        <f>IF(lower!F12=0, "", lower!F12)</f>
-        <v/>
-      </c>
-      <c r="G12" s="63" t="str">
-        <f>IF(lower!$A12=0, "", lower!G12)</f>
+        <f>IF(lower!E12="", "", lower!E12)</f>
+        <v/>
+      </c>
+      <c r="F12" s="69" t="str">
+        <f>IF(lower!F12="", "", lower!F12)</f>
+        <v/>
+      </c>
+      <c r="G12" s="69" t="str">
+        <f>IF(lower!G12="", "", lower!G12)</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="str">
-        <f>IF(lower!A13=0, "", lower!A13)</f>
-        <v/>
-      </c>
-      <c r="B13" s="63" t="str">
-        <f>IF(lower!B13=0, "", lower!B13)</f>
+        <f>IF(lower!A13="", "", lower!A13)</f>
+        <v/>
+      </c>
+      <c r="B13" s="69" t="str">
+        <f>IF(lower!B13="", "", lower!B13)</f>
         <v/>
       </c>
       <c r="C13" s="69" t="str">
-        <f>IF(lower!C13=0, "", lower!C13)</f>
+        <f>IF(lower!C13="", "", lower!C13)</f>
         <v/>
       </c>
       <c r="D13" s="69" t="str">
-        <f>IF(lower!D13=0, "", lower!D13)</f>
+        <f>IF(lower!D13="", "", lower!D13)</f>
         <v/>
       </c>
       <c r="E13" s="69" t="str">
-        <f>IF(lower!E13=0, "", lower!E13)</f>
-        <v/>
-      </c>
-      <c r="F13" s="63" t="str">
-        <f>IF(lower!F13=0, "", lower!F13)</f>
-        <v/>
-      </c>
-      <c r="G13" s="63" t="str">
-        <f>IF(lower!$A13=0, "", lower!G13)</f>
+        <f>IF(lower!E13="", "", lower!E13)</f>
+        <v/>
+      </c>
+      <c r="F13" s="69" t="str">
+        <f>IF(lower!F13="", "", lower!F13)</f>
+        <v/>
+      </c>
+      <c r="G13" s="69" t="str">
+        <f>IF(lower!G13="", "", lower!G13)</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="str">
-        <f>IF(lower!A14=0, "", lower!A14)</f>
+        <f>IF(lower!A14="", "", lower!A14)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B14" s="63">
-        <f>IF(lower!B14=0, "", lower!B14)</f>
+      <c r="B14" s="69">
+        <f>IF(lower!B14="", "", lower!B14)</f>
         <v>9</v>
       </c>
       <c r="C14" s="69">
-        <f>IF(lower!C14=0, "", lower!C14)</f>
+        <f>IF(lower!C14="", "", lower!C14)</f>
         <v>8.12733176437591</v>
       </c>
       <c r="D14" s="69">
-        <f>IF(lower!D14=0, "", lower!D14)</f>
+        <f>IF(lower!D14="", "", lower!D14)</f>
         <v>170.60254037844379</v>
       </c>
       <c r="E14" s="69">
-        <f>IF(lower!E14=0, "", lower!E14)</f>
+        <f>IF(lower!E14="", "", lower!E14)</f>
         <v>89.999859694228434</v>
       </c>
-      <c r="F14" s="63">
-        <f>IF(lower!F14=0, "", lower!F14)</f>
+      <c r="F14" s="69">
+        <f>IF(lower!F14="", "", lower!F14)</f>
         <v>5</v>
       </c>
-      <c r="G14" s="63">
-        <f>IF(lower!$A14=0, "", lower!G14)</f>
+      <c r="G14" s="69">
+        <f>IF(lower!G14="", "", lower!G14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="str">
-        <f>IF(lower!A15=0, "", lower!A15)</f>
+        <f>IF(lower!A15="", "", lower!A15)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B15" s="63">
-        <f>IF(lower!B15=0, "", lower!B15)</f>
+      <c r="B15" s="69">
+        <f>IF(lower!B15="", "", lower!B15)</f>
         <v>6</v>
       </c>
       <c r="C15" s="69">
-        <f>IF(lower!C15=0, "", lower!C15)</f>
+        <f>IF(lower!C15="", "", lower!C15)</f>
         <v>-1.1102725426580946</v>
       </c>
       <c r="D15" s="69">
-        <f>IF(lower!D15=0, "", lower!D15)</f>
+        <f>IF(lower!D15="", "", lower!D15)</f>
         <v>186.60254037844379</v>
       </c>
       <c r="E15" s="69">
-        <f>IF(lower!E15=0, "", lower!E15)</f>
+        <f>IF(lower!E15="", "", lower!E15)</f>
         <v>30</v>
       </c>
-      <c r="F15" s="63">
-        <f>IF(lower!F15=0, "", lower!F15)</f>
+      <c r="F15" s="69">
+        <f>IF(lower!F15="", "", lower!F15)</f>
         <v>5</v>
       </c>
-      <c r="G15" s="63">
-        <f>IF(lower!$A15=0, "", lower!G15)</f>
+      <c r="G15" s="69">
+        <f>IF(lower!G15="", "", lower!G15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="str">
-        <f>IF(lower!A16=0, "", lower!A16)</f>
+        <f>IF(lower!A16="", "", lower!A16)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B16" s="63">
-        <f>IF(lower!B16=0, "", lower!B16)</f>
+      <c r="B16" s="69">
+        <f>IF(lower!B16="", "", lower!B16)</f>
         <v>7</v>
       </c>
       <c r="C16" s="69">
-        <f>IF(lower!C16=0, "", lower!C16)</f>
+        <f>IF(lower!C16="", "", lower!C16)</f>
         <v>8.1273317643759242</v>
       </c>
       <c r="D16" s="69">
-        <f>IF(lower!D16=0, "", lower!D16)</f>
+        <f>IF(lower!D16="", "", lower!D16)</f>
         <v>202.60254037844373</v>
       </c>
       <c r="E16" s="69">
-        <f>IF(lower!E16=0, "", lower!E16)</f>
+        <f>IF(lower!E16="", "", lower!E16)</f>
         <v>-29.999859694228427</v>
       </c>
-      <c r="F16" s="63">
-        <f>IF(lower!F16=0, "", lower!F16)</f>
+      <c r="F16" s="69">
+        <f>IF(lower!F16="", "", lower!F16)</f>
         <v>5</v>
       </c>
-      <c r="G16" s="63">
-        <f>IF(lower!$A16=0, "", lower!G16)</f>
+      <c r="G16" s="69">
+        <f>IF(lower!G16="", "", lower!G16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="str">
-        <f>IF(lower!A17=0, "", lower!A17)</f>
+        <f>IF(lower!A17="", "", lower!A17)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B17" s="63">
-        <f>IF(lower!B17=0, "", lower!B17)</f>
+      <c r="B17" s="69">
+        <f>IF(lower!B17="", "", lower!B17)</f>
         <v>3</v>
       </c>
       <c r="C17" s="69">
-        <f>IF(lower!C17=0, "", lower!C17)</f>
+        <f>IF(lower!C17="", "", lower!C17)</f>
         <v>-19.585481156726104</v>
       </c>
       <c r="D17" s="69">
-        <f>IF(lower!D17=0, "", lower!D17)</f>
+        <f>IF(lower!D17="", "", lower!D17)</f>
         <v>186.60254037844376</v>
       </c>
       <c r="E17" s="69">
-        <f>IF(lower!E17=0, "", lower!E17)</f>
+        <f>IF(lower!E17="", "", lower!E17)</f>
         <v>89.999859694228434</v>
       </c>
-      <c r="F17" s="63">
-        <f>IF(lower!F17=0, "", lower!F17)</f>
+      <c r="F17" s="69">
+        <f>IF(lower!F17="", "", lower!F17)</f>
         <v>5</v>
       </c>
-      <c r="G17" s="63">
-        <f>IF(lower!$A17=0, "", lower!G17)</f>
+      <c r="G17" s="69">
+        <f>IF(lower!G17="", "", lower!G17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="63" t="str">
-        <f>IF(lower!A18=0, "", lower!A18)</f>
+        <f>IF(lower!A18="", "", lower!A18)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B18" s="63">
-        <f>IF(lower!B18=0, "", lower!B18)</f>
+      <c r="B18" s="69">
+        <f>IF(lower!B18="", "", lower!B18)</f>
         <v>4</v>
       </c>
       <c r="C18" s="69">
-        <f>IF(lower!C18=0, "", lower!C18)</f>
+        <f>IF(lower!C18="", "", lower!C18)</f>
         <v>-28.823085463760137</v>
       </c>
       <c r="D18" s="69">
-        <f>IF(lower!D18=0, "", lower!D18)</f>
+        <f>IF(lower!D18="", "", lower!D18)</f>
         <v>170.60254037844379</v>
       </c>
       <c r="E18" s="69">
-        <f>IF(lower!E18=0, "", lower!E18)</f>
+        <f>IF(lower!E18="", "", lower!E18)</f>
         <v>149.99971938845687</v>
       </c>
-      <c r="F18" s="63">
-        <f>IF(lower!F18=0, "", lower!F18)</f>
+      <c r="F18" s="69">
+        <f>IF(lower!F18="", "", lower!F18)</f>
         <v>5</v>
       </c>
-      <c r="G18" s="63">
-        <f>IF(lower!$A18=0, "", lower!G18)</f>
+      <c r="G18" s="69">
+        <f>IF(lower!G18="", "", lower!G18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="63" t="str">
-        <f>IF(lower!A19=0, "", lower!A19)</f>
+        <f>IF(lower!A19="", "", lower!A19)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B19" s="63">
-        <f>IF(lower!B19=0, "", lower!B19)</f>
+      <c r="B19" s="69">
+        <f>IF(lower!B19="", "", lower!B19)</f>
         <v>10</v>
       </c>
       <c r="C19" s="69">
-        <f>IF(lower!C19=0, "", lower!C19)</f>
+        <f>IF(lower!C19="", "", lower!C19)</f>
         <v>-1.1102725426581088</v>
       </c>
       <c r="D19" s="69">
-        <f>IF(lower!D19=0, "", lower!D19)</f>
+        <f>IF(lower!D19="", "", lower!D19)</f>
         <v>154.60254037844382</v>
       </c>
       <c r="E19" s="69">
-        <f>IF(lower!E19=0, "", lower!E19)</f>
+        <f>IF(lower!E19="", "", lower!E19)</f>
         <v>149.99971938845687</v>
       </c>
-      <c r="F19" s="63">
-        <f>IF(lower!F19=0, "", lower!F19)</f>
+      <c r="F19" s="69">
+        <f>IF(lower!F19="", "", lower!F19)</f>
         <v>5</v>
       </c>
-      <c r="G19" s="63">
-        <f>IF(lower!$A19=0, "", lower!G19)</f>
+      <c r="G19" s="69">
+        <f>IF(lower!G19="", "", lower!G19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="str">
-        <f>IF(lower!A20=0, "", lower!A20)</f>
+        <f>IF(lower!A20="", "", lower!A20)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B20" s="63">
-        <f>IF(lower!B20=0, "", lower!B20)</f>
+      <c r="B20" s="69">
+        <f>IF(lower!B20="", "", lower!B20)</f>
         <v>5</v>
       </c>
       <c r="C20" s="69">
-        <f>IF(lower!C20=0, "", lower!C20)</f>
+        <f>IF(lower!C20="", "", lower!C20)</f>
         <v>-19.585481156726132</v>
       </c>
       <c r="D20" s="69">
-        <f>IF(lower!D20=0, "", lower!D20)</f>
+        <f>IF(lower!D20="", "", lower!D20)</f>
         <v>154.60254037844379</v>
       </c>
       <c r="E20" s="69">
-        <f>IF(lower!E20=0, "", lower!E20)</f>
+        <f>IF(lower!E20="", "", lower!E20)</f>
         <v>89.999859694228434</v>
       </c>
-      <c r="F20" s="63">
-        <f>IF(lower!F20=0, "", lower!F20)</f>
+      <c r="F20" s="69">
+        <f>IF(lower!F20="", "", lower!F20)</f>
         <v>5</v>
       </c>
-      <c r="G20" s="63">
-        <f>IF(lower!$A20=0, "", lower!G20)</f>
+      <c r="G20" s="69">
+        <f>IF(lower!G20="", "", lower!G20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="str">
-        <f>IF(lower!A21=0, "", lower!A21)</f>
-        <v/>
-      </c>
-      <c r="B21" s="63" t="str">
-        <f>IF(lower!B21=0, "", lower!B21)</f>
+        <f>IF(lower!A21="", "", lower!A21)</f>
+        <v/>
+      </c>
+      <c r="B21" s="69" t="str">
+        <f>IF(lower!B21="", "", lower!B21)</f>
         <v/>
       </c>
       <c r="C21" s="69" t="str">
-        <f>IF(lower!C21=0, "", lower!C21)</f>
+        <f>IF(lower!C21="", "", lower!C21)</f>
         <v/>
       </c>
       <c r="D21" s="69" t="str">
-        <f>IF(lower!D21=0, "", lower!D21)</f>
+        <f>IF(lower!D21="", "", lower!D21)</f>
         <v/>
       </c>
       <c r="E21" s="69" t="str">
-        <f>IF(lower!E21=0, "", lower!E21)</f>
-        <v/>
-      </c>
-      <c r="F21" s="63" t="str">
-        <f>IF(lower!F21=0, "", lower!F21)</f>
-        <v/>
-      </c>
-      <c r="G21" s="63" t="str">
-        <f>IF(lower!$A21=0, "", lower!G21)</f>
+        <f>IF(lower!E21="", "", lower!E21)</f>
+        <v/>
+      </c>
+      <c r="F21" s="69" t="str">
+        <f>IF(lower!F21="", "", lower!F21)</f>
+        <v/>
+      </c>
+      <c r="G21" s="69" t="str">
+        <f>IF(lower!G21="", "", lower!G21)</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="str">
-        <f>IF(lower!A22=0, "", lower!A22)</f>
-        <v/>
-      </c>
-      <c r="B22" s="63" t="str">
-        <f>IF(lower!B22=0, "", lower!B22)</f>
+        <f>IF(lower!A22="", "", lower!A22)</f>
+        <v/>
+      </c>
+      <c r="B22" s="69" t="str">
+        <f>IF(lower!B22="", "", lower!B22)</f>
         <v/>
       </c>
       <c r="C22" s="69" t="str">
-        <f>IF(lower!C22=0, "", lower!C22)</f>
+        <f>IF(lower!C22="", "", lower!C22)</f>
         <v/>
       </c>
       <c r="D22" s="69" t="str">
-        <f>IF(lower!D22=0, "", lower!D22)</f>
+        <f>IF(lower!D22="", "", lower!D22)</f>
         <v/>
       </c>
       <c r="E22" s="69" t="str">
-        <f>IF(lower!E22=0, "", lower!E22)</f>
-        <v/>
-      </c>
-      <c r="F22" s="63" t="str">
-        <f>IF(lower!F22=0, "", lower!F22)</f>
-        <v/>
-      </c>
-      <c r="G22" s="63" t="str">
-        <f>IF(lower!$A22=0, "", lower!G22)</f>
+        <f>IF(lower!E22="", "", lower!E22)</f>
+        <v/>
+      </c>
+      <c r="F22" s="69" t="str">
+        <f>IF(lower!F22="", "", lower!F22)</f>
+        <v/>
+      </c>
+      <c r="G22" s="69" t="str">
+        <f>IF(lower!G22="", "", lower!G22)</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="str">
-        <f>IF(lower!A23=0, "", lower!A23)</f>
+        <f>IF(lower!A23="", "", lower!A23)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B23" s="63">
-        <f>IF(lower!B23=0, "", lower!B23)</f>
+      <c r="B23" s="69">
+        <f>IF(lower!B23="", "", lower!B23)</f>
         <v>11</v>
       </c>
       <c r="C23" s="69">
-        <f>IF(lower!C23=0, "", lower!C23)</f>
+        <f>IF(lower!C23="", "", lower!C23)</f>
         <v>8.1273317643758958</v>
       </c>
       <c r="D23" s="69">
-        <f>IF(lower!D23=0, "", lower!D23)</f>
+        <f>IF(lower!D23="", "", lower!D23)</f>
         <v>138.60254037844382</v>
       </c>
       <c r="E23" s="69">
-        <f>IF(lower!E23=0, "", lower!E23)</f>
+        <f>IF(lower!E23="", "", lower!E23)</f>
         <v>209.99957908268468</v>
       </c>
-      <c r="F23" s="63">
-        <f>IF(lower!F23=0, "", lower!F23)</f>
+      <c r="F23" s="69">
+        <f>IF(lower!F23="", "", lower!F23)</f>
         <v>5</v>
       </c>
-      <c r="G23" s="63">
-        <f>IF(lower!$A23=0, "", lower!G23)</f>
+      <c r="G23" s="69">
+        <f>IF(lower!G23="", "", lower!G23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="str">
-        <f>IF(lower!A24=0, "", lower!A24)</f>
-        <v/>
-      </c>
-      <c r="B24" s="63" t="str">
-        <f>IF(lower!B24=0, "", lower!B24)</f>
+        <f>IF(lower!A24="", "", lower!A24)</f>
+        <v/>
+      </c>
+      <c r="B24" s="69" t="str">
+        <f>IF(lower!B24="", "", lower!B24)</f>
         <v/>
       </c>
       <c r="C24" s="69" t="str">
-        <f>IF(lower!C24=0, "", lower!C24)</f>
+        <f>IF(lower!C24="", "", lower!C24)</f>
         <v/>
       </c>
       <c r="D24" s="69" t="str">
-        <f>IF(lower!D24=0, "", lower!D24)</f>
+        <f>IF(lower!D24="", "", lower!D24)</f>
         <v/>
       </c>
       <c r="E24" s="69" t="str">
-        <f>IF(lower!E24=0, "", lower!E24)</f>
-        <v/>
-      </c>
-      <c r="F24" s="63" t="str">
-        <f>IF(lower!F24=0, "", lower!F24)</f>
-        <v/>
-      </c>
-      <c r="G24" s="63" t="str">
-        <f>IF(lower!$A24=0, "", lower!G24)</f>
+        <f>IF(lower!E24="", "", lower!E24)</f>
+        <v/>
+      </c>
+      <c r="F24" s="69" t="str">
+        <f>IF(lower!F24="", "", lower!F24)</f>
+        <v/>
+      </c>
+      <c r="G24" s="69" t="str">
+        <f>IF(lower!G24="", "", lower!G24)</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="63" t="str">
-        <f>IF(lower!A25=0, "", lower!A25)</f>
-        <v/>
-      </c>
-      <c r="B25" s="63" t="str">
-        <f>IF(lower!B25=0, "", lower!B25)</f>
+        <f>IF(lower!A25="", "", lower!A25)</f>
+        <v/>
+      </c>
+      <c r="B25" s="69" t="str">
+        <f>IF(lower!B25="", "", lower!B25)</f>
         <v/>
       </c>
       <c r="C25" s="69" t="str">
-        <f>IF(lower!C25=0, "", lower!C25)</f>
+        <f>IF(lower!C25="", "", lower!C25)</f>
         <v/>
       </c>
       <c r="D25" s="69" t="str">
-        <f>IF(lower!D25=0, "", lower!D25)</f>
+        <f>IF(lower!D25="", "", lower!D25)</f>
         <v/>
       </c>
       <c r="E25" s="69" t="str">
-        <f>IF(lower!E25=0, "", lower!E25)</f>
-        <v/>
-      </c>
-      <c r="F25" s="63" t="str">
-        <f>IF(lower!F25=0, "", lower!F25)</f>
-        <v/>
-      </c>
-      <c r="G25" s="63" t="str">
-        <f>IF(lower!$A25=0, "", lower!G25)</f>
+        <f>IF(lower!E25="", "", lower!E25)</f>
+        <v/>
+      </c>
+      <c r="F25" s="69" t="str">
+        <f>IF(lower!F25="", "", lower!F25)</f>
+        <v/>
+      </c>
+      <c r="G25" s="69" t="str">
+        <f>IF(lower!G25="", "", lower!G25)</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="str">
-        <f>IF(external!A3=0, "", external!A3)</f>
+        <f>IF(external!A3="", "", external!A3)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B26" s="62">
-        <f>IF(external!B3=0, "", external!B3)</f>
+      <c r="B26" s="70">
+        <f>IF(external!B3="", "", external!B3)</f>
         <v>16</v>
       </c>
       <c r="C26" s="70">
-        <f>IF(external!C3=0, "", external!C3)</f>
+        <f>IF(external!C3="", "", external!C3)</f>
         <v>86.602540378443877</v>
       </c>
       <c r="D26" s="70">
-        <f>IF(external!D3=0, "", external!D3)</f>
-        <v>136.60254037844388</v>
+        <f>IF(external!D3="", "", external!D3)</f>
+        <v>213.39745962155612</v>
       </c>
       <c r="E26" s="70">
-        <f>IF(external!E3=0, "", external!E3)</f>
-        <v>-89.999719388456853</v>
-      </c>
-      <c r="F26" s="62">
-        <f>IF(external!F3=0, "", external!F3)</f>
+        <f>IF(external!E3="", "", external!E3)</f>
+        <v>149.99971938845687</v>
+      </c>
+      <c r="F26" s="70">
+        <f>IF(external!F3="", "", external!F3)</f>
         <v>5</v>
       </c>
-      <c r="G26" s="62">
-        <f>IF(external!A3=0, "", external!G3)</f>
-        <v>0</v>
+      <c r="G26" s="70">
+        <f>IF(external!G3="", "", external!G3)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="62" t="str">
-        <f>IF(external!A4=0, "", external!A4)</f>
+        <f>IF(external!A4="", "", external!A4)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B27" s="62">
-        <f>IF(external!B4=0, "", external!B4)</f>
+      <c r="B27" s="70">
+        <f>IF(external!B4="", "", external!B4)</f>
         <v>17</v>
       </c>
       <c r="C27" s="70">
-        <f>IF(external!C4=0, "", external!C4)</f>
+        <f>IF(external!C4="", "", external!C4)</f>
         <v>95.840144685477895</v>
       </c>
       <c r="D27" s="70">
-        <f>IF(external!D4=0, "", external!D4)</f>
-        <v>152.60254037844385</v>
+        <f>IF(external!D4="", "", external!D4)</f>
+        <v>197.39745962155615</v>
       </c>
       <c r="E27" s="70">
-        <f>IF(external!E4=0, "", external!E4)</f>
-        <v>-29.999859694228427</v>
-      </c>
-      <c r="F27" s="62">
-        <f>IF(external!F4=0, "", external!F4)</f>
+        <f>IF(external!E4="", "", external!E4)</f>
+        <v>89.999859694228434</v>
+      </c>
+      <c r="F27" s="70">
+        <f>IF(external!F4="", "", external!F4)</f>
         <v>5</v>
       </c>
-      <c r="G27" s="62">
-        <f>IF(external!A4=0, "", external!G4)</f>
-        <v>0</v>
+      <c r="G27" s="70">
+        <f>IF(external!G4="", "", external!G4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="str">
-        <f>IF(external!A5=0, "", external!A5)</f>
-        <v/>
-      </c>
-      <c r="B28" s="62" t="str">
-        <f>IF(external!B5=0, "", external!B5)</f>
+        <f>IF(external!A5="", "", external!A5)</f>
+        <v/>
+      </c>
+      <c r="B28" s="70" t="str">
+        <f>IF(external!B5="", "", external!B5)</f>
         <v/>
       </c>
       <c r="C28" s="70" t="str">
-        <f>IF(external!C5=0, "", external!C5)</f>
+        <f>IF(external!C5="", "", external!C5)</f>
         <v/>
       </c>
       <c r="D28" s="70" t="str">
-        <f>IF(external!D5=0, "", external!D5)</f>
+        <f>IF(external!D5="", "", external!D5)</f>
         <v/>
       </c>
       <c r="E28" s="70" t="str">
-        <f>IF(external!E5=0, "", external!E5)</f>
-        <v/>
-      </c>
-      <c r="F28" s="62" t="str">
-        <f>IF(external!F5=0, "", external!F5)</f>
-        <v/>
-      </c>
-      <c r="G28" s="62" t="str">
-        <f>IF(external!A5=0, "", external!G5)</f>
+        <f>IF(external!E5="", "", external!E5)</f>
+        <v/>
+      </c>
+      <c r="F28" s="70" t="str">
+        <f>IF(external!F5="", "", external!F5)</f>
+        <v/>
+      </c>
+      <c r="G28" s="70" t="str">
+        <f>IF(external!G5="", "", external!G5)</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="62" t="str">
-        <f>IF(external!A6=0, "", external!A6)</f>
-        <v/>
-      </c>
-      <c r="B29" s="62" t="str">
-        <f>IF(external!B6=0, "", external!B6)</f>
+        <f>IF(external!A6="", "", external!A6)</f>
+        <v/>
+      </c>
+      <c r="B29" s="70" t="str">
+        <f>IF(external!B6="", "", external!B6)</f>
         <v/>
       </c>
       <c r="C29" s="70" t="str">
-        <f>IF(external!C6=0, "", external!C6)</f>
+        <f>IF(external!C6="", "", external!C6)</f>
         <v/>
       </c>
       <c r="D29" s="70" t="str">
-        <f>IF(external!D6=0, "", external!D6)</f>
+        <f>IF(external!D6="", "", external!D6)</f>
         <v/>
       </c>
       <c r="E29" s="70" t="str">
-        <f>IF(external!E6=0, "", external!E6)</f>
-        <v/>
-      </c>
-      <c r="F29" s="62" t="str">
-        <f>IF(external!F6=0, "", external!F6)</f>
-        <v/>
-      </c>
-      <c r="G29" s="62" t="str">
-        <f>IF(external!A6=0, "", external!G6)</f>
+        <f>IF(external!E6="", "", external!E6)</f>
+        <v/>
+      </c>
+      <c r="F29" s="70" t="str">
+        <f>IF(external!F6="", "", external!F6)</f>
+        <v/>
+      </c>
+      <c r="G29" s="70" t="str">
+        <f>IF(external!G6="", "", external!G6)</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="str">
-        <f>IF(external!A7=0, "", external!A7)</f>
-        <v/>
-      </c>
-      <c r="B30" s="62" t="str">
-        <f>IF(external!B7=0, "", external!B7)</f>
+        <f>IF(external!A7="", "", external!A7)</f>
+        <v/>
+      </c>
+      <c r="B30" s="70" t="str">
+        <f>IF(external!B7="", "", external!B7)</f>
         <v/>
       </c>
       <c r="C30" s="70" t="str">
-        <f>IF(external!C7=0, "", external!C7)</f>
+        <f>IF(external!C7="", "", external!C7)</f>
         <v/>
       </c>
       <c r="D30" s="70" t="str">
-        <f>IF(external!D7=0, "", external!D7)</f>
+        <f>IF(external!D7="", "", external!D7)</f>
         <v/>
       </c>
       <c r="E30" s="70" t="str">
-        <f>IF(external!E7=0, "", external!E7)</f>
-        <v/>
-      </c>
-      <c r="F30" s="62" t="str">
-        <f>IF(external!F7=0, "", external!F7)</f>
-        <v/>
-      </c>
-      <c r="G30" s="62" t="str">
-        <f>IF(external!A7=0, "", external!G7)</f>
+        <f>IF(external!E7="", "", external!E7)</f>
+        <v/>
+      </c>
+      <c r="F30" s="70" t="str">
+        <f>IF(external!F7="", "", external!F7)</f>
+        <v/>
+      </c>
+      <c r="G30" s="70" t="str">
+        <f>IF(external!G7="", "", external!G7)</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="str">
-        <f>IF(external!A8=0, "", external!A8)</f>
-        <v/>
-      </c>
-      <c r="B31" s="62" t="str">
-        <f>IF(external!B8=0, "", external!B8)</f>
+        <f>IF(external!A8="", "", external!A8)</f>
+        <v/>
+      </c>
+      <c r="B31" s="70" t="str">
+        <f>IF(external!B8="", "", external!B8)</f>
         <v/>
       </c>
       <c r="C31" s="70" t="str">
-        <f>IF(external!C8=0, "", external!C8)</f>
+        <f>IF(external!C8="", "", external!C8)</f>
         <v/>
       </c>
       <c r="D31" s="70" t="str">
-        <f>IF(external!D8=0, "", external!D8)</f>
+        <f>IF(external!D8="", "", external!D8)</f>
         <v/>
       </c>
       <c r="E31" s="70" t="str">
-        <f>IF(external!E8=0, "", external!E8)</f>
-        <v/>
-      </c>
-      <c r="F31" s="62" t="str">
-        <f>IF(external!F8=0, "", external!F8)</f>
-        <v/>
-      </c>
-      <c r="G31" s="62" t="str">
-        <f>IF(external!A8=0, "", external!G8)</f>
+        <f>IF(external!E8="", "", external!E8)</f>
+        <v/>
+      </c>
+      <c r="F31" s="70" t="str">
+        <f>IF(external!F8="", "", external!F8)</f>
+        <v/>
+      </c>
+      <c r="G31" s="70" t="str">
+        <f>IF(external!G8="", "", external!G8)</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="str">
-        <f>IF(external!A9=0, "", external!A9)</f>
-        <v/>
-      </c>
-      <c r="B32" s="62" t="str">
-        <f>IF(external!B9=0, "", external!B9)</f>
+        <f>IF(external!A9="", "", external!A9)</f>
+        <v/>
+      </c>
+      <c r="B32" s="70" t="str">
+        <f>IF(external!B9="", "", external!B9)</f>
         <v/>
       </c>
       <c r="C32" s="70" t="str">
-        <f>IF(external!C9=0, "", external!C9)</f>
+        <f>IF(external!C9="", "", external!C9)</f>
         <v/>
       </c>
       <c r="D32" s="70" t="str">
-        <f>IF(external!D9=0, "", external!D9)</f>
+        <f>IF(external!D9="", "", external!D9)</f>
         <v/>
       </c>
       <c r="E32" s="70" t="str">
-        <f>IF(external!E9=0, "", external!E9)</f>
-        <v/>
-      </c>
-      <c r="F32" s="62" t="str">
-        <f>IF(external!F9=0, "", external!F9)</f>
-        <v/>
-      </c>
-      <c r="G32" s="62" t="str">
-        <f>IF(external!A9=0, "", external!G9)</f>
+        <f>IF(external!E9="", "", external!E9)</f>
+        <v/>
+      </c>
+      <c r="F32" s="70" t="str">
+        <f>IF(external!F9="", "", external!F9)</f>
+        <v/>
+      </c>
+      <c r="G32" s="70" t="str">
+        <f>IF(external!G9="", "", external!G9)</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="str">
-        <f>IF(external!A10=0, "", external!A10)</f>
-        <v/>
-      </c>
-      <c r="B33" s="62" t="str">
-        <f>IF(external!B10=0, "", external!B10)</f>
+        <f>IF(external!A10="", "", external!A10)</f>
+        <v/>
+      </c>
+      <c r="B33" s="70" t="str">
+        <f>IF(external!B10="", "", external!B10)</f>
         <v/>
       </c>
       <c r="C33" s="70" t="str">
-        <f>IF(external!C10=0, "", external!C10)</f>
+        <f>IF(external!C10="", "", external!C10)</f>
         <v/>
       </c>
       <c r="D33" s="70" t="str">
-        <f>IF(external!D10=0, "", external!D10)</f>
+        <f>IF(external!D10="", "", external!D10)</f>
         <v/>
       </c>
       <c r="E33" s="70" t="str">
-        <f>IF(external!E10=0, "", external!E10)</f>
-        <v/>
-      </c>
-      <c r="F33" s="62" t="str">
-        <f>IF(external!F10=0, "", external!F10)</f>
-        <v/>
-      </c>
-      <c r="G33" s="62" t="str">
-        <f>IF(external!A10=0, "", external!G10)</f>
+        <f>IF(external!E10="", "", external!E10)</f>
+        <v/>
+      </c>
+      <c r="F33" s="70" t="str">
+        <f>IF(external!F10="", "", external!F10)</f>
+        <v/>
+      </c>
+      <c r="G33" s="70" t="str">
+        <f>IF(external!G10="", "", external!G10)</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="str">
-        <f>IF(external!A11=0, "", external!A11)</f>
+        <f>IF(external!A11="", "", external!A11)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B34" s="62">
-        <f>IF(external!B11=0, "", external!B11)</f>
+      <c r="B34" s="70">
+        <f>IF(external!B11="", "", external!B11)</f>
         <v>28</v>
       </c>
       <c r="C34" s="70">
-        <f>IF(external!C11=0, "", external!C11)</f>
+        <f>IF(external!C11="", "", external!C11)</f>
         <v>86.602540378443905</v>
       </c>
       <c r="D34" s="70">
-        <f>IF(external!D11=0, "", external!D11)</f>
-        <v>168.60254037844382</v>
+        <f>IF(external!D11="", "", external!D11)</f>
+        <v>181.39745962155618</v>
       </c>
       <c r="E34" s="70">
-        <f>IF(external!E11=0, "", external!E11)</f>
+        <f>IF(external!E11="", "", external!E11)</f>
         <v>30</v>
       </c>
-      <c r="F34" s="62">
-        <f>IF(external!F11=0, "", external!F11)</f>
+      <c r="F34" s="70">
+        <f>IF(external!F11="", "", external!F11)</f>
         <v>5</v>
       </c>
-      <c r="G34" s="62">
-        <f>IF(external!A11=0, "", external!G11)</f>
-        <v>0</v>
+      <c r="G34" s="70">
+        <f>IF(external!G11="", "", external!G11)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="str">
-        <f>IF(external!A12=0, "", external!A12)</f>
+        <f>IF(external!A12="", "", external!A12)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B35" s="62">
-        <f>IF(external!B12=0, "", external!B12)</f>
+      <c r="B35" s="70">
+        <f>IF(external!B12="", "", external!B12)</f>
         <v>29</v>
       </c>
       <c r="C35" s="70">
-        <f>IF(external!C12=0, "", external!C12)</f>
+        <f>IF(external!C12="", "", external!C12)</f>
         <v>95.840144685477924</v>
       </c>
       <c r="D35" s="70">
-        <f>IF(external!D12=0, "", external!D12)</f>
-        <v>184.60254037844379</v>
+        <f>IF(external!D12="", "", external!D12)</f>
+        <v>165.39745962155621</v>
       </c>
       <c r="E35" s="70">
-        <f>IF(external!E12=0, "", external!E12)</f>
-        <v>-29.999859694228427</v>
-      </c>
-      <c r="F35" s="62">
-        <f>IF(external!F12=0, "", external!F12)</f>
+        <f>IF(external!E12="", "", external!E12)</f>
+        <v>89.999859694228434</v>
+      </c>
+      <c r="F35" s="70">
+        <f>IF(external!F12="", "", external!F12)</f>
         <v>5</v>
       </c>
-      <c r="G35" s="62">
-        <f>IF(external!A12=0, "", external!G12)</f>
-        <v>0</v>
+      <c r="G35" s="70">
+        <f>IF(external!G12="", "", external!G12)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="str">
-        <f>IF(external!A13=0, "", external!A13)</f>
+        <f>IF(external!A13="", "", external!A13)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B36" s="62">
-        <f>IF(external!B13=0, "", external!B13)</f>
+      <c r="B36" s="70">
+        <f>IF(external!B13="", "", external!B13)</f>
         <v>24</v>
       </c>
       <c r="C36" s="70">
-        <f>IF(external!C13=0, "", external!C13)</f>
+        <f>IF(external!C13="", "", external!C13)</f>
         <v>86.602540378443919</v>
       </c>
       <c r="D36" s="70">
-        <f>IF(external!D13=0, "", external!D13)</f>
-        <v>200.60254037844379</v>
+        <f>IF(external!D13="", "", external!D13)</f>
+        <v>149.39745962155621</v>
       </c>
       <c r="E36" s="70">
-        <f>IF(external!E13=0, "", external!E13)</f>
+        <f>IF(external!E13="", "", external!E13)</f>
         <v>30</v>
       </c>
-      <c r="F36" s="62">
-        <f>IF(external!F13=0, "", external!F13)</f>
+      <c r="F36" s="70">
+        <f>IF(external!F13="", "", external!F13)</f>
         <v>5</v>
       </c>
-      <c r="G36" s="62">
-        <f>IF(external!A13=0, "", external!G13)</f>
-        <v>0</v>
+      <c r="G36" s="70">
+        <f>IF(external!G13="", "", external!G13)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="str">
-        <f>IF(external!A14=0, "", external!A14)</f>
+        <f>IF(external!A14="", "", external!A14)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B37" s="62">
-        <f>IF(external!B14=0, "", external!B14)</f>
+      <c r="B37" s="70">
+        <f>IF(external!B14="", "", external!B14)</f>
         <v>25</v>
       </c>
       <c r="C37" s="70">
-        <f>IF(external!C14=0, "", external!C14)</f>
+        <f>IF(external!C14="", "", external!C14)</f>
         <v>68.12733176437591</v>
       </c>
       <c r="D37" s="70">
-        <f>IF(external!D14=0, "", external!D14)</f>
-        <v>200.60254037844379</v>
+        <f>IF(external!D14="", "", external!D14)</f>
+        <v>149.39745962155621</v>
       </c>
       <c r="E37" s="70">
-        <f>IF(external!E14=0, "", external!E14)</f>
-        <v>89.999859694228434</v>
-      </c>
-      <c r="F37" s="62">
-        <f>IF(external!F14=0, "", external!F14)</f>
+        <f>IF(external!E14="", "", external!E14)</f>
+        <v>-29.999859694228427</v>
+      </c>
+      <c r="F37" s="70">
+        <f>IF(external!F14="", "", external!F14)</f>
         <v>5</v>
       </c>
-      <c r="G37" s="62">
-        <f>IF(external!A14=0, "", external!G14)</f>
-        <v>0</v>
+      <c r="G37" s="70">
+        <f>IF(external!G14="", "", external!G14)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="62" t="str">
-        <f>IF(external!A15=0, "", external!A15)</f>
+        <f>IF(external!A15="", "", external!A15)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B38" s="62">
-        <f>IF(external!B15=0, "", external!B15)</f>
+      <c r="B38" s="70">
+        <f>IF(external!B15="", "", external!B15)</f>
         <v>22</v>
       </c>
       <c r="C38" s="70">
-        <f>IF(external!C15=0, "", external!C15)</f>
+        <f>IF(external!C15="", "", external!C15)</f>
         <v>58.889727457341905</v>
       </c>
       <c r="D38" s="70">
-        <f>IF(external!D15=0, "", external!D15)</f>
-        <v>216.60254037844379</v>
+        <f>IF(external!D15="", "", external!D15)</f>
+        <v>133.39745962155621</v>
       </c>
       <c r="E38" s="70">
-        <f>IF(external!E15=0, "", external!E15)</f>
+        <f>IF(external!E15="", "", external!E15)</f>
         <v>30</v>
       </c>
-      <c r="F38" s="62">
-        <f>IF(external!F15=0, "", external!F15)</f>
+      <c r="F38" s="70">
+        <f>IF(external!F15="", "", external!F15)</f>
         <v>5</v>
       </c>
-      <c r="G38" s="62">
-        <f>IF(external!A15=0, "", external!G15)</f>
-        <v>0</v>
+      <c r="G38" s="70">
+        <f>IF(external!G15="", "", external!G15)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="62" t="str">
-        <f>IF(external!A16=0, "", external!A16)</f>
-        <v/>
-      </c>
-      <c r="B39" s="62" t="str">
-        <f>IF(external!B16=0, "", external!B16)</f>
+        <f>IF(external!A16="", "", external!A16)</f>
+        <v/>
+      </c>
+      <c r="B39" s="70" t="str">
+        <f>IF(external!B16="", "", external!B16)</f>
         <v/>
       </c>
       <c r="C39" s="70" t="str">
-        <f>IF(external!C16=0, "", external!C16)</f>
+        <f>IF(external!C16="", "", external!C16)</f>
         <v/>
       </c>
       <c r="D39" s="70" t="str">
-        <f>IF(external!D16=0, "", external!D16)</f>
+        <f>IF(external!D16="", "", external!D16)</f>
         <v/>
       </c>
       <c r="E39" s="70" t="str">
-        <f>IF(external!E16=0, "", external!E16)</f>
-        <v/>
-      </c>
-      <c r="F39" s="62" t="str">
-        <f>IF(external!F16=0, "", external!F16)</f>
-        <v/>
-      </c>
-      <c r="G39" s="62" t="str">
-        <f>IF(external!A16=0, "", external!G16)</f>
+        <f>IF(external!E16="", "", external!E16)</f>
+        <v/>
+      </c>
+      <c r="F39" s="70" t="str">
+        <f>IF(external!F16="", "", external!F16)</f>
+        <v/>
+      </c>
+      <c r="G39" s="70" t="str">
+        <f>IF(external!G16="", "", external!G16)</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="62" t="str">
-        <f>IF(external!A17=0, "", external!A17)</f>
-        <v/>
-      </c>
-      <c r="B40" s="62" t="str">
-        <f>IF(external!B17=0, "", external!B17)</f>
+        <f>IF(external!A17="", "", external!A17)</f>
+        <v/>
+      </c>
+      <c r="B40" s="70" t="str">
+        <f>IF(external!B17="", "", external!B17)</f>
         <v/>
       </c>
       <c r="C40" s="70" t="str">
-        <f>IF(external!C17=0, "", external!C17)</f>
+        <f>IF(external!C17="", "", external!C17)</f>
         <v/>
       </c>
       <c r="D40" s="70" t="str">
-        <f>IF(external!D17=0, "", external!D17)</f>
+        <f>IF(external!D17="", "", external!D17)</f>
         <v/>
       </c>
       <c r="E40" s="70" t="str">
-        <f>IF(external!E17=0, "", external!E17)</f>
-        <v/>
-      </c>
-      <c r="F40" s="62" t="str">
-        <f>IF(external!F17=0, "", external!F17)</f>
-        <v/>
-      </c>
-      <c r="G40" s="62" t="str">
-        <f>IF(external!A17=0, "", external!G17)</f>
+        <f>IF(external!E17="", "", external!E17)</f>
+        <v/>
+      </c>
+      <c r="F40" s="70" t="str">
+        <f>IF(external!F17="", "", external!F17)</f>
+        <v/>
+      </c>
+      <c r="G40" s="70" t="str">
+        <f>IF(external!G17="", "", external!G17)</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="str">
-        <f>IF(external!A18=0, "", external!A18)</f>
-        <v/>
-      </c>
-      <c r="B41" s="62" t="str">
-        <f>IF(external!B18=0, "", external!B18)</f>
+        <f>IF(external!A18="", "", external!A18)</f>
+        <v/>
+      </c>
+      <c r="B41" s="70" t="str">
+        <f>IF(external!B18="", "", external!B18)</f>
         <v/>
       </c>
       <c r="C41" s="70" t="str">
-        <f>IF(external!C18=0, "", external!C18)</f>
+        <f>IF(external!C18="", "", external!C18)</f>
         <v/>
       </c>
       <c r="D41" s="70" t="str">
-        <f>IF(external!D18=0, "", external!D18)</f>
+        <f>IF(external!D18="", "", external!D18)</f>
         <v/>
       </c>
       <c r="E41" s="70" t="str">
-        <f>IF(external!E18=0, "", external!E18)</f>
-        <v/>
-      </c>
-      <c r="F41" s="62" t="str">
-        <f>IF(external!F18=0, "", external!F18)</f>
-        <v/>
-      </c>
-      <c r="G41" s="62" t="str">
-        <f>IF(external!A18=0, "", external!G18)</f>
+        <f>IF(external!E18="", "", external!E18)</f>
+        <v/>
+      </c>
+      <c r="F41" s="70" t="str">
+        <f>IF(external!F18="", "", external!F18)</f>
+        <v/>
+      </c>
+      <c r="G41" s="70" t="str">
+        <f>IF(external!G18="", "", external!G18)</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="str">
-        <f>IF(external!A19=0, "", external!A19)</f>
+        <f>IF(external!A19="", "", external!A19)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B42" s="62">
-        <f>IF(external!B19=0, "", external!B19)</f>
+      <c r="B42" s="70">
+        <f>IF(external!B19="", "", external!B19)</f>
         <v>26</v>
       </c>
       <c r="C42" s="70">
-        <f>IF(external!C19=0, "", external!C19)</f>
+        <f>IF(external!C19="", "", external!C19)</f>
         <v>58.889727457341891</v>
       </c>
       <c r="D42" s="70">
-        <f>IF(external!D19=0, "", external!D19)</f>
-        <v>184.60254037844382</v>
+        <f>IF(external!D19="", "", external!D19)</f>
+        <v>165.39745962155618</v>
       </c>
       <c r="E42" s="70">
-        <f>IF(external!E19=0, "", external!E19)</f>
-        <v>149.99971938845687</v>
-      </c>
-      <c r="F42" s="62">
-        <f>IF(external!F19=0, "", external!F19)</f>
+        <f>IF(external!E19="", "", external!E19)</f>
+        <v>-89.999719388456853</v>
+      </c>
+      <c r="F42" s="70">
+        <f>IF(external!F19="", "", external!F19)</f>
         <v>5</v>
       </c>
-      <c r="G42" s="62">
-        <f>IF(external!A19=0, "", external!G19)</f>
-        <v>0</v>
+      <c r="G42" s="70">
+        <f>IF(external!G19="", "", external!G19)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="62" t="str">
-        <f>IF(external!A20=0, "", external!A20)</f>
-        <v/>
-      </c>
-      <c r="B43" s="62" t="str">
-        <f>IF(external!B20=0, "", external!B20)</f>
+        <f>IF(external!A20="", "", external!A20)</f>
+        <v/>
+      </c>
+      <c r="B43" s="70" t="str">
+        <f>IF(external!B20="", "", external!B20)</f>
         <v/>
       </c>
       <c r="C43" s="70" t="str">
-        <f>IF(external!C20=0, "", external!C20)</f>
+        <f>IF(external!C20="", "", external!C20)</f>
         <v/>
       </c>
       <c r="D43" s="70" t="str">
-        <f>IF(external!D20=0, "", external!D20)</f>
+        <f>IF(external!D20="", "", external!D20)</f>
         <v/>
       </c>
       <c r="E43" s="70" t="str">
-        <f>IF(external!E20=0, "", external!E20)</f>
-        <v/>
-      </c>
-      <c r="F43" s="62" t="str">
-        <f>IF(external!F20=0, "", external!F20)</f>
-        <v/>
-      </c>
-      <c r="G43" s="62" t="str">
-        <f>IF(external!A20=0, "", external!G20)</f>
+        <f>IF(external!E20="", "", external!E20)</f>
+        <v/>
+      </c>
+      <c r="F43" s="70" t="str">
+        <f>IF(external!F20="", "", external!F20)</f>
+        <v/>
+      </c>
+      <c r="G43" s="70" t="str">
+        <f>IF(external!G20="", "", external!G20)</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="62" t="str">
-        <f>IF(external!A21=0, "", external!A21)</f>
-        <v/>
-      </c>
-      <c r="B44" s="62" t="str">
-        <f>IF(external!B21=0, "", external!B21)</f>
+        <f>IF(external!A21="", "", external!A21)</f>
+        <v/>
+      </c>
+      <c r="B44" s="70" t="str">
+        <f>IF(external!B21="", "", external!B21)</f>
         <v/>
       </c>
       <c r="C44" s="70" t="str">
-        <f>IF(external!C21=0, "", external!C21)</f>
+        <f>IF(external!C21="", "", external!C21)</f>
         <v/>
       </c>
       <c r="D44" s="70" t="str">
-        <f>IF(external!D21=0, "", external!D21)</f>
+        <f>IF(external!D21="", "", external!D21)</f>
         <v/>
       </c>
       <c r="E44" s="70" t="str">
-        <f>IF(external!E21=0, "", external!E21)</f>
-        <v/>
-      </c>
-      <c r="F44" s="62" t="str">
-        <f>IF(external!F21=0, "", external!F21)</f>
-        <v/>
-      </c>
-      <c r="G44" s="62" t="str">
-        <f>IF(external!A21=0, "", external!G21)</f>
+        <f>IF(external!E21="", "", external!E21)</f>
+        <v/>
+      </c>
+      <c r="F44" s="70" t="str">
+        <f>IF(external!F21="", "", external!F21)</f>
+        <v/>
+      </c>
+      <c r="G44" s="70" t="str">
+        <f>IF(external!G21="", "", external!G21)</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="62" t="str">
-        <f>IF(external!A22=0, "", external!A22)</f>
-        <v/>
-      </c>
-      <c r="B45" s="62" t="str">
-        <f>IF(external!B22=0, "", external!B22)</f>
+        <f>IF(external!A22="", "", external!A22)</f>
+        <v/>
+      </c>
+      <c r="B45" s="70" t="str">
+        <f>IF(external!B22="", "", external!B22)</f>
         <v/>
       </c>
       <c r="C45" s="70" t="str">
-        <f>IF(external!C22=0, "", external!C22)</f>
+        <f>IF(external!C22="", "", external!C22)</f>
         <v/>
       </c>
       <c r="D45" s="70" t="str">
-        <f>IF(external!D22=0, "", external!D22)</f>
+        <f>IF(external!D22="", "", external!D22)</f>
         <v/>
       </c>
       <c r="E45" s="70" t="str">
-        <f>IF(external!E22=0, "", external!E22)</f>
-        <v/>
-      </c>
-      <c r="F45" s="62" t="str">
-        <f>IF(external!F22=0, "", external!F22)</f>
-        <v/>
-      </c>
-      <c r="G45" s="62" t="str">
-        <f>IF(external!A22=0, "", external!G22)</f>
+        <f>IF(external!E22="", "", external!E22)</f>
+        <v/>
+      </c>
+      <c r="F45" s="70" t="str">
+        <f>IF(external!F22="", "", external!F22)</f>
+        <v/>
+      </c>
+      <c r="G45" s="70" t="str">
+        <f>IF(external!G22="", "", external!G22)</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="62" t="str">
-        <f>IF(external!A23=0, "", external!A23)</f>
+        <f>IF(external!A23="", "", external!A23)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B46" s="62">
-        <f>IF(external!B23=0, "", external!B23)</f>
+      <c r="B46" s="70">
+        <f>IF(external!B23="", "", external!B23)</f>
         <v>27</v>
       </c>
       <c r="C46" s="70">
-        <f>IF(external!C23=0, "", external!C23)</f>
+        <f>IF(external!C23="", "", external!C23)</f>
         <v>68.127331764375896</v>
       </c>
       <c r="D46" s="70">
-        <f>IF(external!D23=0, "", external!D23)</f>
-        <v>168.60254037844382</v>
+        <f>IF(external!D23="", "", external!D23)</f>
+        <v>181.39745962155618</v>
       </c>
       <c r="E46" s="70">
-        <f>IF(external!E23=0, "", external!E23)</f>
-        <v>209.99957908268468</v>
-      </c>
-      <c r="F46" s="62">
-        <f>IF(external!F23=0, "", external!F23)</f>
+        <f>IF(external!E23="", "", external!E23)</f>
+        <v>-149.99957908268468</v>
+      </c>
+      <c r="F46" s="70">
+        <f>IF(external!F23="", "", external!F23)</f>
         <v>5</v>
       </c>
-      <c r="G46" s="62">
-        <f>IF(external!A23=0, "", external!G23)</f>
-        <v>0</v>
+      <c r="G46" s="70">
+        <f>IF(external!G23="", "", external!G23)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="62" t="str">
-        <f>IF(external!A24=0, "", external!A24)</f>
+        <f>IF(external!A24="", "", external!A24)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B47" s="62">
-        <f>IF(external!B24=0, "", external!B24)</f>
+      <c r="B47" s="70">
+        <f>IF(external!B24="", "", external!B24)</f>
         <v>30</v>
       </c>
       <c r="C47" s="70">
-        <f>IF(external!C24=0, "", external!C24)</f>
+        <f>IF(external!C24="", "", external!C24)</f>
         <v>58.889727457341856</v>
       </c>
       <c r="D47" s="70">
-        <f>IF(external!D24=0, "", external!D24)</f>
-        <v>152.60254037844382</v>
+        <f>IF(external!D24="", "", external!D24)</f>
+        <v>197.39745962155618</v>
       </c>
       <c r="E47" s="70">
-        <f>IF(external!E24=0, "", external!E24)</f>
-        <v>149.99971938845687</v>
-      </c>
-      <c r="F47" s="62">
-        <f>IF(external!F24=0, "", external!F24)</f>
+        <f>IF(external!E24="", "", external!E24)</f>
+        <v>-89.999719388456853</v>
+      </c>
+      <c r="F47" s="70">
+        <f>IF(external!F24="", "", external!F24)</f>
         <v>5</v>
       </c>
-      <c r="G47" s="62">
-        <f>IF(external!A24=0, "", external!G24)</f>
-        <v>0</v>
+      <c r="G47" s="70">
+        <f>IF(external!G24="", "", external!G24)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="62" t="str">
-        <f>IF(external!A25=0, "", external!A25)</f>
+        <f>IF(external!A25="", "", external!A25)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B48" s="62">
-        <f>IF(external!B25=0, "", external!B25)</f>
+      <c r="B48" s="70">
+        <f>IF(external!B25="", "", external!B25)</f>
         <v>31</v>
       </c>
       <c r="C48" s="70">
-        <f>IF(external!C25=0, "", external!C25)</f>
+        <f>IF(external!C25="", "", external!C25)</f>
         <v>68.127331764375853</v>
       </c>
       <c r="D48" s="70">
-        <f>IF(external!D25=0, "", external!D25)</f>
-        <v>136.60254037844385</v>
+        <f>IF(external!D25="", "", external!D25)</f>
+        <v>213.39745962155615</v>
       </c>
       <c r="E48" s="70">
-        <f>IF(external!E25=0, "", external!E25)</f>
-        <v>209.99957908268468</v>
-      </c>
-      <c r="F48" s="62">
-        <f>IF(external!F25=0, "", external!F25)</f>
+        <f>IF(external!E25="", "", external!E25)</f>
+        <v>-149.99957908268468</v>
+      </c>
+      <c r="F48" s="70">
+        <f>IF(external!F25="", "", external!F25)</f>
         <v>5</v>
       </c>
-      <c r="G48" s="62">
-        <f>IF(external!A25=0, "", external!G25)</f>
-        <v>0</v>
+      <c r="G48" s="70">
+        <f>IF(external!G25="", "", external!G25)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="61" t="str">
-        <f>IF(internal!A3=0, "", internal!A3)</f>
+        <f>IF(internal!A3="", "", internal!A3)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B49" s="61">
-        <f>IF(internal!B3=0, "", internal!B3)</f>
+      <c r="B49" s="71">
+        <f>IF(internal!B3="", "", internal!B3)</f>
         <v>32</v>
       </c>
       <c r="C49" s="71">
-        <f>IF(internal!C3=0, "", internal!C3)</f>
+        <f>IF(internal!C3="", "", internal!C3)</f>
         <v>-76.602540378443848</v>
       </c>
       <c r="D49" s="71">
-        <f>IF(internal!D3=0, "", internal!D3)</f>
-        <v>213.39745962155612</v>
+        <f>IF(internal!D3="", "", internal!D3)</f>
+        <v>136.60254037844388</v>
       </c>
       <c r="E49" s="71">
-        <f>IF(internal!E3=0, "", internal!E3)</f>
-        <v>90.000280611543147</v>
-      </c>
-      <c r="F49" s="61">
-        <f>IF(internal!F3=0, "", internal!F3)</f>
+        <f>IF(internal!E3="", "", internal!E3)</f>
+        <v>329.99971938845687</v>
+      </c>
+      <c r="F49" s="71">
+        <f>IF(internal!F3="", "", internal!F3)</f>
         <v>5</v>
       </c>
-      <c r="G49" s="61">
-        <f>IF(internal!A3=0, "", internal!G3)</f>
-        <v>0</v>
+      <c r="G49" s="71">
+        <f>IF(internal!G3="", "", internal!G3)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="61" t="str">
-        <f>IF(internal!A4=0, "", internal!A4)</f>
+        <f>IF(internal!A4="", "", internal!A4)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B50" s="61">
-        <f>IF(internal!B4=0, "", internal!B4)</f>
+      <c r="B50" s="71">
+        <f>IF(internal!B4="", "", internal!B4)</f>
         <v>33</v>
       </c>
       <c r="C50" s="71">
-        <f>IF(internal!C4=0, "", internal!C4)</f>
+        <f>IF(internal!C4="", "", internal!C4)</f>
         <v>-85.840144685477867</v>
       </c>
       <c r="D50" s="71">
-        <f>IF(internal!D4=0, "", internal!D4)</f>
-        <v>197.39745962155615</v>
+        <f>IF(internal!D4="", "", internal!D4)</f>
+        <v>152.60254037844385</v>
       </c>
       <c r="E50" s="71">
-        <f>IF(internal!E4=0, "", internal!E4)</f>
-        <v>150.00014030577157</v>
-      </c>
-      <c r="F50" s="61">
-        <f>IF(internal!F4=0, "", internal!F4)</f>
+        <f>IF(internal!E4="", "", internal!E4)</f>
+        <v>269.99985969422841</v>
+      </c>
+      <c r="F50" s="71">
+        <f>IF(internal!F4="", "", internal!F4)</f>
         <v>5</v>
       </c>
-      <c r="G50" s="61">
-        <f>IF(internal!A4=0, "", internal!G4)</f>
-        <v>0</v>
+      <c r="G50" s="71">
+        <f>IF(internal!G4="", "", internal!G4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="61" t="str">
-        <f>IF(internal!A5=0, "", internal!A5)</f>
+        <f>IF(internal!A5="", "", internal!A5)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B51" s="61">
-        <f>IF(internal!B5=0, "", internal!B5)</f>
+      <c r="B51" s="71">
+        <f>IF(internal!B5="", "", internal!B5)</f>
         <v>34</v>
       </c>
       <c r="C51" s="71">
-        <f>IF(internal!C5=0, "", internal!C5)</f>
+        <f>IF(internal!C5="", "", internal!C5)</f>
         <v>-104.31535329954588</v>
       </c>
       <c r="D51" s="71">
-        <f>IF(internal!D5=0, "", internal!D5)</f>
-        <v>197.39745962155612</v>
+        <f>IF(internal!D5="", "", internal!D5)</f>
+        <v>152.60254037844388</v>
       </c>
       <c r="E51" s="71">
-        <f>IF(internal!E5=0, "", internal!E5)</f>
-        <v>90.000280611543147</v>
-      </c>
-      <c r="F51" s="61">
-        <f>IF(internal!F5=0, "", internal!F5)</f>
+        <f>IF(internal!E5="", "", internal!E5)</f>
+        <v>329.99971938845687</v>
+      </c>
+      <c r="F51" s="71">
+        <f>IF(internal!F5="", "", internal!F5)</f>
         <v>5</v>
       </c>
-      <c r="G51" s="61">
-        <f>IF(internal!A5=0, "", internal!G5)</f>
-        <v>0</v>
+      <c r="G51" s="71">
+        <f>IF(internal!G5="", "", internal!G5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="61" t="str">
-        <f>IF(internal!A6=0, "", internal!A6)</f>
+        <f>IF(internal!A6="", "", internal!A6)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B52" s="61">
-        <f>IF(internal!B6=0, "", internal!B6)</f>
+      <c r="B52" s="71">
+        <f>IF(internal!B6="", "", internal!B6)</f>
         <v>35</v>
       </c>
       <c r="C52" s="71">
-        <f>IF(internal!C6=0, "", internal!C6)</f>
+        <f>IF(internal!C6="", "", internal!C6)</f>
         <v>-113.55295760657989</v>
       </c>
       <c r="D52" s="71">
-        <f>IF(internal!D6=0, "", internal!D6)</f>
-        <v>181.39745962155615</v>
+        <f>IF(internal!D6="", "", internal!D6)</f>
+        <v>168.60254037844385</v>
       </c>
       <c r="E52" s="71">
-        <f>IF(internal!E6=0, "", internal!E6)</f>
-        <v>150.00014030577157</v>
-      </c>
-      <c r="F52" s="61">
-        <f>IF(internal!F6=0, "", internal!F6)</f>
+        <f>IF(internal!E6="", "", internal!E6)</f>
+        <v>269.99985969422841</v>
+      </c>
+      <c r="F52" s="71">
+        <f>IF(internal!F6="", "", internal!F6)</f>
         <v>5</v>
       </c>
-      <c r="G52" s="61">
-        <f>IF(internal!A6=0, "", internal!G6)</f>
-        <v>0</v>
+      <c r="G52" s="71">
+        <f>IF(internal!G6="", "", internal!G6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="61" t="str">
-        <f>IF(internal!A7=0, "", internal!A7)</f>
+        <f>IF(internal!A7="", "", internal!A7)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B53" s="61">
-        <f>IF(internal!B7=0, "", internal!B7)</f>
+      <c r="B53" s="71">
+        <f>IF(internal!B7="", "", internal!B7)</f>
         <v>36</v>
       </c>
       <c r="C53" s="71">
-        <f>IF(internal!C7=0, "", internal!C7)</f>
+        <f>IF(internal!C7="", "", internal!C7)</f>
         <v>-104.31535329954589</v>
       </c>
       <c r="D53" s="71">
-        <f>IF(internal!D7=0, "", internal!D7)</f>
-        <v>165.39745962155615</v>
+        <f>IF(internal!D7="", "", internal!D7)</f>
+        <v>184.60254037844385</v>
       </c>
       <c r="E53" s="71">
-        <f>IF(internal!E7=0, "", internal!E7)</f>
+        <f>IF(internal!E7="", "", internal!E7)</f>
         <v>210</v>
       </c>
-      <c r="F53" s="61">
-        <f>IF(internal!F7=0, "", internal!F7)</f>
+      <c r="F53" s="71">
+        <f>IF(internal!F7="", "", internal!F7)</f>
         <v>5</v>
       </c>
-      <c r="G53" s="61">
-        <f>IF(internal!A7=0, "", internal!G7)</f>
-        <v>0</v>
+      <c r="G53" s="71">
+        <f>IF(internal!G7="", "", internal!G7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="61" t="str">
-        <f>IF(internal!A8=0, "", internal!A8)</f>
+        <f>IF(internal!A8="", "", internal!A8)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B54" s="61">
-        <f>IF(internal!B8=0, "", internal!B8)</f>
+      <c r="B54" s="71">
+        <f>IF(internal!B8="", "", internal!B8)</f>
         <v>37</v>
       </c>
       <c r="C54" s="71">
-        <f>IF(internal!C8=0, "", internal!C8)</f>
+        <f>IF(internal!C8="", "", internal!C8)</f>
         <v>-113.55295760657992</v>
       </c>
       <c r="D54" s="71">
-        <f>IF(internal!D8=0, "", internal!D8)</f>
-        <v>149.39745962155618</v>
+        <f>IF(internal!D8="", "", internal!D8)</f>
+        <v>200.60254037844382</v>
       </c>
       <c r="E54" s="71">
-        <f>IF(internal!E8=0, "", internal!E8)</f>
-        <v>150.00014030577157</v>
-      </c>
-      <c r="F54" s="61">
-        <f>IF(internal!F8=0, "", internal!F8)</f>
+        <f>IF(internal!E8="", "", internal!E8)</f>
+        <v>269.99985969422841</v>
+      </c>
+      <c r="F54" s="71">
+        <f>IF(internal!F8="", "", internal!F8)</f>
         <v>5</v>
       </c>
-      <c r="G54" s="61">
-        <f>IF(internal!A8=0, "", internal!G8)</f>
-        <v>0</v>
+      <c r="G54" s="71">
+        <f>IF(internal!G8="", "", internal!G8)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="61" t="str">
-        <f>IF(internal!A9=0, "", internal!A9)</f>
+        <f>IF(internal!A9="", "", internal!A9)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B55" s="61">
-        <f>IF(internal!B9=0, "", internal!B9)</f>
+      <c r="B55" s="71">
+        <f>IF(internal!B9="", "", internal!B9)</f>
         <v>38</v>
       </c>
       <c r="C55" s="71">
-        <f>IF(internal!C9=0, "", internal!C9)</f>
+        <f>IF(internal!C9="", "", internal!C9)</f>
         <v>-104.31535329954592</v>
       </c>
       <c r="D55" s="71">
-        <f>IF(internal!D9=0, "", internal!D9)</f>
-        <v>133.39745962155621</v>
+        <f>IF(internal!D9="", "", internal!D9)</f>
+        <v>216.60254037844379</v>
       </c>
       <c r="E55" s="71">
-        <f>IF(internal!E9=0, "", internal!E9)</f>
+        <f>IF(internal!E9="", "", internal!E9)</f>
         <v>210</v>
       </c>
-      <c r="F55" s="61">
-        <f>IF(internal!F9=0, "", internal!F9)</f>
+      <c r="F55" s="71">
+        <f>IF(internal!F9="", "", internal!F9)</f>
         <v>5</v>
       </c>
-      <c r="G55" s="61">
-        <f>IF(internal!A9=0, "", internal!G9)</f>
-        <v>0</v>
+      <c r="G55" s="71">
+        <f>IF(internal!G9="", "", internal!G9)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="61" t="str">
-        <f>IF(internal!A10=0, "", internal!A10)</f>
+        <f>IF(internal!A10="", "", internal!A10)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B56" s="61">
-        <f>IF(internal!B10=0, "", internal!B10)</f>
+      <c r="B56" s="71">
+        <f>IF(internal!B10="", "", internal!B10)</f>
         <v>39</v>
       </c>
       <c r="C56" s="71">
-        <f>IF(internal!C10=0, "", internal!C10)</f>
+        <f>IF(internal!C10="", "", internal!C10)</f>
         <v>-85.840144685477895</v>
       </c>
       <c r="D56" s="71">
-        <f>IF(internal!D10=0, "", internal!D10)</f>
-        <v>133.39745962155621</v>
+        <f>IF(internal!D10="", "", internal!D10)</f>
+        <v>216.60254037844379</v>
       </c>
       <c r="E56" s="71">
-        <f>IF(internal!E10=0, "", internal!E10)</f>
-        <v>269.99985969422841</v>
-      </c>
-      <c r="F56" s="61">
-        <f>IF(internal!F10=0, "", internal!F10)</f>
+        <f>IF(internal!E10="", "", internal!E10)</f>
+        <v>150.00014030577157</v>
+      </c>
+      <c r="F56" s="71">
+        <f>IF(internal!F10="", "", internal!F10)</f>
         <v>5</v>
       </c>
-      <c r="G56" s="61">
-        <f>IF(internal!A10=0, "", internal!G10)</f>
-        <v>0</v>
+      <c r="G56" s="71">
+        <f>IF(internal!G10="", "", internal!G10)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="61" t="str">
-        <f>IF(internal!A11=0, "", internal!A11)</f>
+        <f>IF(internal!A11="", "", internal!A11)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B57" s="61">
-        <f>IF(internal!B11=0, "", internal!B11)</f>
+      <c r="B57" s="71">
+        <f>IF(internal!B11="", "", internal!B11)</f>
         <v>44</v>
       </c>
       <c r="C57" s="71">
-        <f>IF(internal!C11=0, "", internal!C11)</f>
+        <f>IF(internal!C11="", "", internal!C11)</f>
         <v>-76.602540378443862</v>
       </c>
       <c r="D57" s="71">
-        <f>IF(internal!D11=0, "", internal!D11)</f>
-        <v>181.39745962155615</v>
+        <f>IF(internal!D11="", "", internal!D11)</f>
+        <v>168.60254037844385</v>
       </c>
       <c r="E57" s="71">
-        <f>IF(internal!E11=0, "", internal!E11)</f>
+        <f>IF(internal!E11="", "", internal!E11)</f>
         <v>210</v>
       </c>
-      <c r="F57" s="61">
-        <f>IF(internal!F11=0, "", internal!F11)</f>
+      <c r="F57" s="71">
+        <f>IF(internal!F11="", "", internal!F11)</f>
         <v>5</v>
       </c>
-      <c r="G57" s="61">
-        <f>IF(internal!A11=0, "", internal!G11)</f>
-        <v>0</v>
+      <c r="G57" s="71">
+        <f>IF(internal!G11="", "", internal!G11)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="61" t="str">
-        <f>IF(internal!A12=0, "", internal!A12)</f>
+        <f>IF(internal!A12="", "", internal!A12)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B58" s="61">
-        <f>IF(internal!B12=0, "", internal!B12)</f>
+      <c r="B58" s="71">
+        <f>IF(internal!B12="", "", internal!B12)</f>
         <v>45</v>
       </c>
       <c r="C58" s="71">
-        <f>IF(internal!C12=0, "", internal!C12)</f>
+        <f>IF(internal!C12="", "", internal!C12)</f>
         <v>-85.840144685477881</v>
       </c>
       <c r="D58" s="71">
-        <f>IF(internal!D12=0, "", internal!D12)</f>
-        <v>165.39745962155618</v>
+        <f>IF(internal!D12="", "", internal!D12)</f>
+        <v>184.60254037844382</v>
       </c>
       <c r="E58" s="71">
-        <f>IF(internal!E12=0, "", internal!E12)</f>
-        <v>150.00014030577157</v>
-      </c>
-      <c r="F58" s="61">
-        <f>IF(internal!F12=0, "", internal!F12)</f>
+        <f>IF(internal!E12="", "", internal!E12)</f>
+        <v>269.99985969422841</v>
+      </c>
+      <c r="F58" s="71">
+        <f>IF(internal!F12="", "", internal!F12)</f>
         <v>5</v>
       </c>
-      <c r="G58" s="61">
-        <f>IF(internal!A12=0, "", internal!G12)</f>
-        <v>0</v>
+      <c r="G58" s="71">
+        <f>IF(internal!G12="", "", internal!G12)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="61" t="str">
-        <f>IF(internal!A13=0, "", internal!A13)</f>
+        <f>IF(internal!A13="", "", internal!A13)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B59" s="61">
-        <f>IF(internal!B13=0, "", internal!B13)</f>
+      <c r="B59" s="71">
+        <f>IF(internal!B13="", "", internal!B13)</f>
         <v>40</v>
       </c>
       <c r="C59" s="71">
-        <f>IF(internal!C13=0, "", internal!C13)</f>
+        <f>IF(internal!C13="", "", internal!C13)</f>
         <v>-76.602540378443877</v>
       </c>
       <c r="D59" s="71">
-        <f>IF(internal!D13=0, "", internal!D13)</f>
-        <v>149.39745962155621</v>
+        <f>IF(internal!D13="", "", internal!D13)</f>
+        <v>200.60254037844379</v>
       </c>
       <c r="E59" s="71">
-        <f>IF(internal!E13=0, "", internal!E13)</f>
+        <f>IF(internal!E13="", "", internal!E13)</f>
         <v>210</v>
       </c>
-      <c r="F59" s="61">
-        <f>IF(internal!F13=0, "", internal!F13)</f>
+      <c r="F59" s="71">
+        <f>IF(internal!F13="", "", internal!F13)</f>
         <v>5</v>
       </c>
-      <c r="G59" s="61">
-        <f>IF(internal!A13=0, "", internal!G13)</f>
-        <v>0</v>
+      <c r="G59" s="71">
+        <f>IF(internal!G13="", "", internal!G13)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="61" t="str">
-        <f>IF(internal!A14=0, "", internal!A14)</f>
-        <v/>
-      </c>
-      <c r="B60" s="61" t="str">
-        <f>IF(internal!B14=0, "", internal!B14)</f>
+        <f>IF(internal!A14="", "", internal!A14)</f>
+        <v/>
+      </c>
+      <c r="B60" s="71" t="str">
+        <f>IF(internal!B14="", "", internal!B14)</f>
         <v/>
       </c>
       <c r="C60" s="71" t="str">
-        <f>IF(internal!C14=0, "", internal!C14)</f>
+        <f>IF(internal!C14="", "", internal!C14)</f>
         <v/>
       </c>
       <c r="D60" s="71" t="str">
-        <f>IF(internal!D14=0, "", internal!D14)</f>
+        <f>IF(internal!D14="", "", internal!D14)</f>
         <v/>
       </c>
       <c r="E60" s="71" t="str">
-        <f>IF(internal!E14=0, "", internal!E14)</f>
-        <v/>
-      </c>
-      <c r="F60" s="61" t="str">
-        <f>IF(internal!F14=0, "", internal!F14)</f>
-        <v/>
-      </c>
-      <c r="G60" s="61" t="str">
-        <f>IF(internal!A14=0, "", internal!G14)</f>
+        <f>IF(internal!E14="", "", internal!E14)</f>
+        <v/>
+      </c>
+      <c r="F60" s="71" t="str">
+        <f>IF(internal!F14="", "", internal!F14)</f>
+        <v/>
+      </c>
+      <c r="G60" s="71" t="str">
+        <f>IF(internal!G14="", "", internal!G14)</f>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="61" t="str">
-        <f>IF(internal!A15=0, "", internal!A15)</f>
-        <v/>
-      </c>
-      <c r="B61" s="61" t="str">
-        <f>IF(internal!B15=0, "", internal!B15)</f>
+        <f>IF(internal!A15="", "", internal!A15)</f>
+        <v/>
+      </c>
+      <c r="B61" s="71" t="str">
+        <f>IF(internal!B15="", "", internal!B15)</f>
         <v/>
       </c>
       <c r="C61" s="71" t="str">
-        <f>IF(internal!C15=0, "", internal!C15)</f>
+        <f>IF(internal!C15="", "", internal!C15)</f>
         <v/>
       </c>
       <c r="D61" s="71" t="str">
-        <f>IF(internal!D15=0, "", internal!D15)</f>
+        <f>IF(internal!D15="", "", internal!D15)</f>
         <v/>
       </c>
       <c r="E61" s="71" t="str">
-        <f>IF(internal!E15=0, "", internal!E15)</f>
-        <v/>
-      </c>
-      <c r="F61" s="61" t="str">
-        <f>IF(internal!F15=0, "", internal!F15)</f>
-        <v/>
-      </c>
-      <c r="G61" s="61" t="str">
-        <f>IF(internal!A15=0, "", internal!G15)</f>
+        <f>IF(internal!E15="", "", internal!E15)</f>
+        <v/>
+      </c>
+      <c r="F61" s="71" t="str">
+        <f>IF(internal!F15="", "", internal!F15)</f>
+        <v/>
+      </c>
+      <c r="G61" s="71" t="str">
+        <f>IF(internal!G15="", "", internal!G15)</f>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="61" t="str">
-        <f>IF(internal!A16=0, "", internal!A16)</f>
-        <v/>
-      </c>
-      <c r="B62" s="61" t="str">
-        <f>IF(internal!B16=0, "", internal!B16)</f>
+        <f>IF(internal!A16="", "", internal!A16)</f>
+        <v/>
+      </c>
+      <c r="B62" s="71" t="str">
+        <f>IF(internal!B16="", "", internal!B16)</f>
         <v/>
       </c>
       <c r="C62" s="71" t="str">
-        <f>IF(internal!C16=0, "", internal!C16)</f>
+        <f>IF(internal!C16="", "", internal!C16)</f>
         <v/>
       </c>
       <c r="D62" s="71" t="str">
-        <f>IF(internal!D16=0, "", internal!D16)</f>
+        <f>IF(internal!D16="", "", internal!D16)</f>
         <v/>
       </c>
       <c r="E62" s="71" t="str">
-        <f>IF(internal!E16=0, "", internal!E16)</f>
-        <v/>
-      </c>
-      <c r="F62" s="61" t="str">
-        <f>IF(internal!F16=0, "", internal!F16)</f>
-        <v/>
-      </c>
-      <c r="G62" s="61" t="str">
-        <f>IF(internal!A16=0, "", internal!G16)</f>
+        <f>IF(internal!E16="", "", internal!E16)</f>
+        <v/>
+      </c>
+      <c r="F62" s="71" t="str">
+        <f>IF(internal!F16="", "", internal!F16)</f>
+        <v/>
+      </c>
+      <c r="G62" s="71" t="str">
+        <f>IF(internal!G16="", "", internal!G16)</f>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="61" t="str">
-        <f>IF(internal!A17=0, "", internal!A17)</f>
-        <v/>
-      </c>
-      <c r="B63" s="61" t="str">
-        <f>IF(internal!B17=0, "", internal!B17)</f>
+        <f>IF(internal!A17="", "", internal!A17)</f>
+        <v/>
+      </c>
+      <c r="B63" s="71" t="str">
+        <f>IF(internal!B17="", "", internal!B17)</f>
         <v/>
       </c>
       <c r="C63" s="71" t="str">
-        <f>IF(internal!C17=0, "", internal!C17)</f>
+        <f>IF(internal!C17="", "", internal!C17)</f>
         <v/>
       </c>
       <c r="D63" s="71" t="str">
-        <f>IF(internal!D17=0, "", internal!D17)</f>
+        <f>IF(internal!D17="", "", internal!D17)</f>
         <v/>
       </c>
       <c r="E63" s="71" t="str">
-        <f>IF(internal!E17=0, "", internal!E17)</f>
-        <v/>
-      </c>
-      <c r="F63" s="61" t="str">
-        <f>IF(internal!F17=0, "", internal!F17)</f>
-        <v/>
-      </c>
-      <c r="G63" s="61" t="str">
-        <f>IF(internal!A17=0, "", internal!G17)</f>
+        <f>IF(internal!E17="", "", internal!E17)</f>
+        <v/>
+      </c>
+      <c r="F63" s="71" t="str">
+        <f>IF(internal!F17="", "", internal!F17)</f>
+        <v/>
+      </c>
+      <c r="G63" s="71" t="str">
+        <f>IF(internal!G17="", "", internal!G17)</f>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="61" t="str">
-        <f>IF(internal!A18=0, "", internal!A18)</f>
-        <v/>
-      </c>
-      <c r="B64" s="61" t="str">
-        <f>IF(internal!B18=0, "", internal!B18)</f>
+        <f>IF(internal!A18="", "", internal!A18)</f>
+        <v/>
+      </c>
+      <c r="B64" s="71" t="str">
+        <f>IF(internal!B18="", "", internal!B18)</f>
         <v/>
       </c>
       <c r="C64" s="71" t="str">
-        <f>IF(internal!C18=0, "", internal!C18)</f>
+        <f>IF(internal!C18="", "", internal!C18)</f>
         <v/>
       </c>
       <c r="D64" s="71" t="str">
-        <f>IF(internal!D18=0, "", internal!D18)</f>
+        <f>IF(internal!D18="", "", internal!D18)</f>
         <v/>
       </c>
       <c r="E64" s="71" t="str">
-        <f>IF(internal!E18=0, "", internal!E18)</f>
-        <v/>
-      </c>
-      <c r="F64" s="61" t="str">
-        <f>IF(internal!F18=0, "", internal!F18)</f>
-        <v/>
-      </c>
-      <c r="G64" s="61" t="str">
-        <f>IF(internal!A18=0, "", internal!G18)</f>
+        <f>IF(internal!E18="", "", internal!E18)</f>
+        <v/>
+      </c>
+      <c r="F64" s="71" t="str">
+        <f>IF(internal!F18="", "", internal!F18)</f>
+        <v/>
+      </c>
+      <c r="G64" s="71" t="str">
+        <f>IF(internal!G18="", "", internal!G18)</f>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="61" t="str">
-        <f>IF(internal!A19=0, "", internal!A19)</f>
-        <v/>
-      </c>
-      <c r="B65" s="61" t="str">
-        <f>IF(internal!B19=0, "", internal!B19)</f>
+        <f>IF(internal!A19="", "", internal!A19)</f>
+        <v/>
+      </c>
+      <c r="B65" s="71" t="str">
+        <f>IF(internal!B19="", "", internal!B19)</f>
         <v/>
       </c>
       <c r="C65" s="71" t="str">
-        <f>IF(internal!C19=0, "", internal!C19)</f>
+        <f>IF(internal!C19="", "", internal!C19)</f>
         <v/>
       </c>
       <c r="D65" s="71" t="str">
-        <f>IF(internal!D19=0, "", internal!D19)</f>
+        <f>IF(internal!D19="", "", internal!D19)</f>
         <v/>
       </c>
       <c r="E65" s="71" t="str">
-        <f>IF(internal!E19=0, "", internal!E19)</f>
-        <v/>
-      </c>
-      <c r="F65" s="61" t="str">
-        <f>IF(internal!F19=0, "", internal!F19)</f>
-        <v/>
-      </c>
-      <c r="G65" s="61" t="str">
-        <f>IF(internal!A19=0, "", internal!G19)</f>
+        <f>IF(internal!E19="", "", internal!E19)</f>
+        <v/>
+      </c>
+      <c r="F65" s="71" t="str">
+        <f>IF(internal!F19="", "", internal!F19)</f>
+        <v/>
+      </c>
+      <c r="G65" s="71" t="str">
+        <f>IF(internal!G19="", "", internal!G19)</f>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="61" t="str">
-        <f>IF(internal!A20=0, "", internal!A20)</f>
-        <v/>
-      </c>
-      <c r="B66" s="61" t="str">
-        <f>IF(internal!B20=0, "", internal!B20)</f>
+        <f>IF(internal!A20="", "", internal!A20)</f>
+        <v/>
+      </c>
+      <c r="B66" s="71" t="str">
+        <f>IF(internal!B20="", "", internal!B20)</f>
         <v/>
       </c>
       <c r="C66" s="71" t="str">
-        <f>IF(internal!C20=0, "", internal!C20)</f>
+        <f>IF(internal!C20="", "", internal!C20)</f>
         <v/>
       </c>
       <c r="D66" s="71" t="str">
-        <f>IF(internal!D20=0, "", internal!D20)</f>
+        <f>IF(internal!D20="", "", internal!D20)</f>
         <v/>
       </c>
       <c r="E66" s="71" t="str">
-        <f>IF(internal!E20=0, "", internal!E20)</f>
-        <v/>
-      </c>
-      <c r="F66" s="61" t="str">
-        <f>IF(internal!F20=0, "", internal!F20)</f>
-        <v/>
-      </c>
-      <c r="G66" s="61" t="str">
-        <f>IF(internal!A20=0, "", internal!G20)</f>
+        <f>IF(internal!E20="", "", internal!E20)</f>
+        <v/>
+      </c>
+      <c r="F66" s="71" t="str">
+        <f>IF(internal!F20="", "", internal!F20)</f>
+        <v/>
+      </c>
+      <c r="G66" s="71" t="str">
+        <f>IF(internal!G20="", "", internal!G20)</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="61" t="str">
-        <f>IF(internal!A21=0, "", internal!A21)</f>
-        <v/>
-      </c>
-      <c r="B67" s="61" t="str">
-        <f>IF(internal!B21=0, "", internal!B21)</f>
+        <f>IF(internal!A21="", "", internal!A21)</f>
+        <v/>
+      </c>
+      <c r="B67" s="71" t="str">
+        <f>IF(internal!B21="", "", internal!B21)</f>
         <v/>
       </c>
       <c r="C67" s="71" t="str">
-        <f>IF(internal!C21=0, "", internal!C21)</f>
+        <f>IF(internal!C21="", "", internal!C21)</f>
         <v/>
       </c>
       <c r="D67" s="71" t="str">
-        <f>IF(internal!D21=0, "", internal!D21)</f>
+        <f>IF(internal!D21="", "", internal!D21)</f>
         <v/>
       </c>
       <c r="E67" s="71" t="str">
-        <f>IF(internal!E21=0, "", internal!E21)</f>
-        <v/>
-      </c>
-      <c r="F67" s="61" t="str">
-        <f>IF(internal!F21=0, "", internal!F21)</f>
-        <v/>
-      </c>
-      <c r="G67" s="61" t="str">
-        <f>IF(internal!A21=0, "", internal!G21)</f>
+        <f>IF(internal!E21="", "", internal!E21)</f>
+        <v/>
+      </c>
+      <c r="F67" s="71" t="str">
+        <f>IF(internal!F21="", "", internal!F21)</f>
+        <v/>
+      </c>
+      <c r="G67" s="71" t="str">
+        <f>IF(internal!G21="", "", internal!G21)</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="61" t="str">
-        <f>IF(internal!A22=0, "", internal!A22)</f>
-        <v/>
-      </c>
-      <c r="B68" s="61" t="str">
-        <f>IF(internal!B22=0, "", internal!B22)</f>
+        <f>IF(internal!A22="", "", internal!A22)</f>
+        <v/>
+      </c>
+      <c r="B68" s="71" t="str">
+        <f>IF(internal!B22="", "", internal!B22)</f>
         <v/>
       </c>
       <c r="C68" s="71" t="str">
-        <f>IF(internal!C22=0, "", internal!C22)</f>
+        <f>IF(internal!C22="", "", internal!C22)</f>
         <v/>
       </c>
       <c r="D68" s="71" t="str">
-        <f>IF(internal!D22=0, "", internal!D22)</f>
+        <f>IF(internal!D22="", "", internal!D22)</f>
         <v/>
       </c>
       <c r="E68" s="71" t="str">
-        <f>IF(internal!E22=0, "", internal!E22)</f>
-        <v/>
-      </c>
-      <c r="F68" s="61" t="str">
-        <f>IF(internal!F22=0, "", internal!F22)</f>
-        <v/>
-      </c>
-      <c r="G68" s="61" t="str">
-        <f>IF(internal!A22=0, "", internal!G22)</f>
+        <f>IF(internal!E22="", "", internal!E22)</f>
+        <v/>
+      </c>
+      <c r="F68" s="71" t="str">
+        <f>IF(internal!F22="", "", internal!F22)</f>
+        <v/>
+      </c>
+      <c r="G68" s="71" t="str">
+        <f>IF(internal!G22="", "", internal!G22)</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="61" t="str">
-        <f>IF(internal!A23=0, "", internal!A23)</f>
-        <v/>
-      </c>
-      <c r="B69" s="61" t="str">
-        <f>IF(internal!B23=0, "", internal!B23)</f>
+        <f>IF(internal!A23="", "", internal!A23)</f>
+        <v/>
+      </c>
+      <c r="B69" s="71" t="str">
+        <f>IF(internal!B23="", "", internal!B23)</f>
         <v/>
       </c>
       <c r="C69" s="71" t="str">
-        <f>IF(internal!C23=0, "", internal!C23)</f>
+        <f>IF(internal!C23="", "", internal!C23)</f>
         <v/>
       </c>
       <c r="D69" s="71" t="str">
-        <f>IF(internal!D23=0, "", internal!D23)</f>
+        <f>IF(internal!D23="", "", internal!D23)</f>
         <v/>
       </c>
       <c r="E69" s="71" t="str">
-        <f>IF(internal!E23=0, "", internal!E23)</f>
-        <v/>
-      </c>
-      <c r="F69" s="61" t="str">
-        <f>IF(internal!F23=0, "", internal!F23)</f>
-        <v/>
-      </c>
-      <c r="G69" s="61" t="str">
-        <f>IF(internal!A23=0, "", internal!G23)</f>
+        <f>IF(internal!E23="", "", internal!E23)</f>
+        <v/>
+      </c>
+      <c r="F69" s="71" t="str">
+        <f>IF(internal!F23="", "", internal!F23)</f>
+        <v/>
+      </c>
+      <c r="G69" s="71" t="str">
+        <f>IF(internal!G23="", "", internal!G23)</f>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="61" t="str">
-        <f>IF(internal!A24=0, "", internal!A24)</f>
-        <v/>
-      </c>
-      <c r="B70" s="61" t="str">
-        <f>IF(internal!B24=0, "", internal!B24)</f>
+        <f>IF(internal!A24="", "", internal!A24)</f>
+        <v/>
+      </c>
+      <c r="B70" s="71" t="str">
+        <f>IF(internal!B24="", "", internal!B24)</f>
         <v/>
       </c>
       <c r="C70" s="71" t="str">
-        <f>IF(internal!C24=0, "", internal!C24)</f>
+        <f>IF(internal!C24="", "", internal!C24)</f>
         <v/>
       </c>
       <c r="D70" s="71" t="str">
-        <f>IF(internal!D24=0, "", internal!D24)</f>
+        <f>IF(internal!D24="", "", internal!D24)</f>
         <v/>
       </c>
       <c r="E70" s="71" t="str">
-        <f>IF(internal!E24=0, "", internal!E24)</f>
-        <v/>
-      </c>
-      <c r="F70" s="61" t="str">
-        <f>IF(internal!F24=0, "", internal!F24)</f>
-        <v/>
-      </c>
-      <c r="G70" s="61" t="str">
-        <f>IF(internal!A24=0, "", internal!G24)</f>
+        <f>IF(internal!E24="", "", internal!E24)</f>
+        <v/>
+      </c>
+      <c r="F70" s="71" t="str">
+        <f>IF(internal!F24="", "", internal!F24)</f>
+        <v/>
+      </c>
+      <c r="G70" s="71" t="str">
+        <f>IF(internal!G24="", "", internal!G24)</f>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="61" t="str">
-        <f>IF(internal!A25=0, "", internal!A25)</f>
-        <v/>
-      </c>
-      <c r="B71" s="61" t="str">
-        <f>IF(internal!B25=0, "", internal!B25)</f>
+        <f>IF(internal!A25="", "", internal!A25)</f>
+        <v/>
+      </c>
+      <c r="B71" s="71" t="str">
+        <f>IF(internal!B25="", "", internal!B25)</f>
         <v/>
       </c>
       <c r="C71" s="71" t="str">
-        <f>IF(internal!C25=0, "", internal!C25)</f>
+        <f>IF(internal!C25="", "", internal!C25)</f>
         <v/>
       </c>
       <c r="D71" s="71" t="str">
-        <f>IF(internal!D25=0, "", internal!D25)</f>
+        <f>IF(internal!D25="", "", internal!D25)</f>
         <v/>
       </c>
       <c r="E71" s="71" t="str">
-        <f>IF(internal!E25=0, "", internal!E25)</f>
-        <v/>
-      </c>
-      <c r="F71" s="61" t="str">
-        <f>IF(internal!F25=0, "", internal!F25)</f>
-        <v/>
-      </c>
-      <c r="G71" s="61" t="str">
-        <f>IF(internal!A25=0, "", internal!G25)</f>
+        <f>IF(internal!E25="", "", internal!E25)</f>
+        <v/>
+      </c>
+      <c r="F71" s="71" t="str">
+        <f>IF(internal!F25="", "", internal!F25)</f>
+        <v/>
+      </c>
+      <c r="G71" s="71" t="str">
+        <f>IF(internal!G25="", "", internal!G25)</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="64" t="str">
-        <f>IF(upper!A3=0, "", upper!A3)</f>
-        <v/>
-      </c>
-      <c r="B72" s="64" t="str">
-        <f>IF(upper!B3=0, "", upper!B3)</f>
+        <f>IF(upper!A3="", "", upper!A3)</f>
+        <v/>
+      </c>
+      <c r="B72" s="72" t="str">
+        <f>IF(upper!B3="", "", upper!B3)</f>
         <v/>
       </c>
       <c r="C72" s="72" t="str">
-        <f>IF(upper!C3=0, "", upper!C3)</f>
+        <f>IF(upper!C3="", "", upper!C3)</f>
         <v/>
       </c>
       <c r="D72" s="72" t="str">
-        <f>IF(upper!D3=0, "", upper!D3)</f>
+        <f>IF(upper!D3="", "", upper!D3)</f>
         <v/>
       </c>
       <c r="E72" s="72" t="str">
-        <f>IF(upper!E3=0, "", upper!E3)</f>
-        <v/>
-      </c>
-      <c r="F72" s="64" t="str">
-        <f>IF(upper!F3=0, "", upper!F3)</f>
-        <v/>
-      </c>
-      <c r="G72" s="64" t="str">
-        <f>IF(upper!A3=0, "", upper!G3)</f>
+        <f>IF(upper!E3="", "", upper!E3)</f>
+        <v/>
+      </c>
+      <c r="F72" s="72" t="str">
+        <f>IF(upper!F3="", "", upper!F3)</f>
+        <v/>
+      </c>
+      <c r="G72" s="72" t="str">
+        <f>IF(upper!G3="", "", upper!G3)</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="64" t="str">
-        <f>IF(upper!A4=0, "", upper!A4)</f>
-        <v/>
-      </c>
-      <c r="B73" s="64" t="str">
-        <f>IF(upper!B4=0, "", upper!B4)</f>
+        <f>IF(upper!A4="", "", upper!A4)</f>
+        <v/>
+      </c>
+      <c r="B73" s="72" t="str">
+        <f>IF(upper!B4="", "", upper!B4)</f>
         <v/>
       </c>
       <c r="C73" s="72" t="str">
-        <f>IF(upper!C4=0, "", upper!C4)</f>
+        <f>IF(upper!C4="", "", upper!C4)</f>
         <v/>
       </c>
       <c r="D73" s="72" t="str">
-        <f>IF(upper!D4=0, "", upper!D4)</f>
+        <f>IF(upper!D4="", "", upper!D4)</f>
         <v/>
       </c>
       <c r="E73" s="72" t="str">
-        <f>IF(upper!E4=0, "", upper!E4)</f>
-        <v/>
-      </c>
-      <c r="F73" s="64" t="str">
-        <f>IF(upper!F4=0, "", upper!F4)</f>
-        <v/>
-      </c>
-      <c r="G73" s="64" t="str">
-        <f>IF(upper!A4=0, "", upper!G4)</f>
+        <f>IF(upper!E4="", "", upper!E4)</f>
+        <v/>
+      </c>
+      <c r="F73" s="72" t="str">
+        <f>IF(upper!F4="", "", upper!F4)</f>
+        <v/>
+      </c>
+      <c r="G73" s="72" t="str">
+        <f>IF(upper!G4="", "", upper!G4)</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="64" t="str">
-        <f>IF(upper!A5=0, "", upper!A5)</f>
-        <v/>
-      </c>
-      <c r="B74" s="64" t="str">
-        <f>IF(upper!B5=0, "", upper!B5)</f>
+        <f>IF(upper!A5="", "", upper!A5)</f>
+        <v/>
+      </c>
+      <c r="B74" s="72" t="str">
+        <f>IF(upper!B5="", "", upper!B5)</f>
         <v/>
       </c>
       <c r="C74" s="72" t="str">
-        <f>IF(upper!C5=0, "", upper!C5)</f>
+        <f>IF(upper!C5="", "", upper!C5)</f>
         <v/>
       </c>
       <c r="D74" s="72" t="str">
-        <f>IF(upper!D5=0, "", upper!D5)</f>
+        <f>IF(upper!D5="", "", upper!D5)</f>
         <v/>
       </c>
       <c r="E74" s="72" t="str">
-        <f>IF(upper!E5=0, "", upper!E5)</f>
-        <v/>
-      </c>
-      <c r="F74" s="64" t="str">
-        <f>IF(upper!F5=0, "", upper!F5)</f>
-        <v/>
-      </c>
-      <c r="G74" s="64" t="str">
-        <f>IF(upper!A5=0, "", upper!G5)</f>
+        <f>IF(upper!E5="", "", upper!E5)</f>
+        <v/>
+      </c>
+      <c r="F74" s="72" t="str">
+        <f>IF(upper!F5="", "", upper!F5)</f>
+        <v/>
+      </c>
+      <c r="G74" s="72" t="str">
+        <f>IF(upper!G5="", "", upper!G5)</f>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="64" t="str">
-        <f>IF(upper!A6=0, "", upper!A6)</f>
-        <v/>
-      </c>
-      <c r="B75" s="64" t="str">
-        <f>IF(upper!B6=0, "", upper!B6)</f>
+        <f>IF(upper!A6="", "", upper!A6)</f>
+        <v/>
+      </c>
+      <c r="B75" s="72" t="str">
+        <f>IF(upper!B6="", "", upper!B6)</f>
         <v/>
       </c>
       <c r="C75" s="72" t="str">
-        <f>IF(upper!C6=0, "", upper!C6)</f>
+        <f>IF(upper!C6="", "", upper!C6)</f>
         <v/>
       </c>
       <c r="D75" s="72" t="str">
-        <f>IF(upper!D6=0, "", upper!D6)</f>
+        <f>IF(upper!D6="", "", upper!D6)</f>
         <v/>
       </c>
       <c r="E75" s="72" t="str">
-        <f>IF(upper!E6=0, "", upper!E6)</f>
-        <v/>
-      </c>
-      <c r="F75" s="64" t="str">
-        <f>IF(upper!F6=0, "", upper!F6)</f>
-        <v/>
-      </c>
-      <c r="G75" s="64" t="str">
-        <f>IF(upper!A6=0, "", upper!G6)</f>
+        <f>IF(upper!E6="", "", upper!E6)</f>
+        <v/>
+      </c>
+      <c r="F75" s="72" t="str">
+        <f>IF(upper!F6="", "", upper!F6)</f>
+        <v/>
+      </c>
+      <c r="G75" s="72" t="str">
+        <f>IF(upper!G6="", "", upper!G6)</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="64" t="str">
-        <f>IF(upper!A7=0, "", upper!A7)</f>
-        <v/>
-      </c>
-      <c r="B76" s="64" t="str">
-        <f>IF(upper!B7=0, "", upper!B7)</f>
+        <f>IF(upper!A7="", "", upper!A7)</f>
+        <v/>
+      </c>
+      <c r="B76" s="72" t="str">
+        <f>IF(upper!B7="", "", upper!B7)</f>
         <v/>
       </c>
       <c r="C76" s="72" t="str">
-        <f>IF(upper!C7=0, "", upper!C7)</f>
+        <f>IF(upper!C7="", "", upper!C7)</f>
         <v/>
       </c>
       <c r="D76" s="72" t="str">
-        <f>IF(upper!D7=0, "", upper!D7)</f>
+        <f>IF(upper!D7="", "", upper!D7)</f>
         <v/>
       </c>
       <c r="E76" s="72" t="str">
-        <f>IF(upper!E7=0, "", upper!E7)</f>
-        <v/>
-      </c>
-      <c r="F76" s="64" t="str">
-        <f>IF(upper!F7=0, "", upper!F7)</f>
-        <v/>
-      </c>
-      <c r="G76" s="64" t="str">
-        <f>IF(upper!A7=0, "", upper!G7)</f>
+        <f>IF(upper!E7="", "", upper!E7)</f>
+        <v/>
+      </c>
+      <c r="F76" s="72" t="str">
+        <f>IF(upper!F7="", "", upper!F7)</f>
+        <v/>
+      </c>
+      <c r="G76" s="72" t="str">
+        <f>IF(upper!G7="", "", upper!G7)</f>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="64" t="str">
-        <f>IF(upper!A8=0, "", upper!A8)</f>
-        <v/>
-      </c>
-      <c r="B77" s="64" t="str">
-        <f>IF(upper!B8=0, "", upper!B8)</f>
+        <f>IF(upper!A8="", "", upper!A8)</f>
+        <v/>
+      </c>
+      <c r="B77" s="72" t="str">
+        <f>IF(upper!B8="", "", upper!B8)</f>
         <v/>
       </c>
       <c r="C77" s="72" t="str">
-        <f>IF(upper!C8=0, "", upper!C8)</f>
+        <f>IF(upper!C8="", "", upper!C8)</f>
         <v/>
       </c>
       <c r="D77" s="72" t="str">
-        <f>IF(upper!D8=0, "", upper!D8)</f>
+        <f>IF(upper!D8="", "", upper!D8)</f>
         <v/>
       </c>
       <c r="E77" s="72" t="str">
-        <f>IF(upper!E8=0, "", upper!E8)</f>
-        <v/>
-      </c>
-      <c r="F77" s="64" t="str">
-        <f>IF(upper!F8=0, "", upper!F8)</f>
-        <v/>
-      </c>
-      <c r="G77" s="64" t="str">
-        <f>IF(upper!A8=0, "", upper!G8)</f>
+        <f>IF(upper!E8="", "", upper!E8)</f>
+        <v/>
+      </c>
+      <c r="F77" s="72" t="str">
+        <f>IF(upper!F8="", "", upper!F8)</f>
+        <v/>
+      </c>
+      <c r="G77" s="72" t="str">
+        <f>IF(upper!G8="", "", upper!G8)</f>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="64" t="str">
-        <f>IF(upper!A9=0, "", upper!A9)</f>
-        <v/>
-      </c>
-      <c r="B78" s="64" t="str">
-        <f>IF(upper!B9=0, "", upper!B9)</f>
+        <f>IF(upper!A9="", "", upper!A9)</f>
+        <v/>
+      </c>
+      <c r="B78" s="72" t="str">
+        <f>IF(upper!B9="", "", upper!B9)</f>
         <v/>
       </c>
       <c r="C78" s="72" t="str">
-        <f>IF(upper!C9=0, "", upper!C9)</f>
+        <f>IF(upper!C9="", "", upper!C9)</f>
         <v/>
       </c>
       <c r="D78" s="72" t="str">
-        <f>IF(upper!D9=0, "", upper!D9)</f>
+        <f>IF(upper!D9="", "", upper!D9)</f>
         <v/>
       </c>
       <c r="E78" s="72" t="str">
-        <f>IF(upper!E9=0, "", upper!E9)</f>
-        <v/>
-      </c>
-      <c r="F78" s="64" t="str">
-        <f>IF(upper!F9=0, "", upper!F9)</f>
-        <v/>
-      </c>
-      <c r="G78" s="64" t="str">
-        <f>IF(upper!A9=0, "", upper!G9)</f>
+        <f>IF(upper!E9="", "", upper!E9)</f>
+        <v/>
+      </c>
+      <c r="F78" s="72" t="str">
+        <f>IF(upper!F9="", "", upper!F9)</f>
+        <v/>
+      </c>
+      <c r="G78" s="72" t="str">
+        <f>IF(upper!G9="", "", upper!G9)</f>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="64" t="str">
-        <f>IF(upper!A10=0, "", upper!A10)</f>
-        <v/>
-      </c>
-      <c r="B79" s="64" t="str">
-        <f>IF(upper!B10=0, "", upper!B10)</f>
+        <f>IF(upper!A10="", "", upper!A10)</f>
+        <v/>
+      </c>
+      <c r="B79" s="72" t="str">
+        <f>IF(upper!B10="", "", upper!B10)</f>
         <v/>
       </c>
       <c r="C79" s="72" t="str">
-        <f>IF(upper!C10=0, "", upper!C10)</f>
+        <f>IF(upper!C10="", "", upper!C10)</f>
         <v/>
       </c>
       <c r="D79" s="72" t="str">
-        <f>IF(upper!D10=0, "", upper!D10)</f>
+        <f>IF(upper!D10="", "", upper!D10)</f>
         <v/>
       </c>
       <c r="E79" s="72" t="str">
-        <f>IF(upper!E10=0, "", upper!E10)</f>
-        <v/>
-      </c>
-      <c r="F79" s="64" t="str">
-        <f>IF(upper!F10=0, "", upper!F10)</f>
-        <v/>
-      </c>
-      <c r="G79" s="64" t="str">
-        <f>IF(upper!A10=0, "", upper!G10)</f>
+        <f>IF(upper!E10="", "", upper!E10)</f>
+        <v/>
+      </c>
+      <c r="F79" s="72" t="str">
+        <f>IF(upper!F10="", "", upper!F10)</f>
+        <v/>
+      </c>
+      <c r="G79" s="72" t="str">
+        <f>IF(upper!G10="", "", upper!G10)</f>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="64" t="str">
-        <f>IF(upper!A11=0, "", upper!A11)</f>
-        <v/>
-      </c>
-      <c r="B80" s="64" t="str">
-        <f>IF(upper!B11=0, "", upper!B11)</f>
+        <f>IF(upper!A11="", "", upper!A11)</f>
+        <v/>
+      </c>
+      <c r="B80" s="72" t="str">
+        <f>IF(upper!B11="", "", upper!B11)</f>
         <v/>
       </c>
       <c r="C80" s="72" t="str">
-        <f>IF(upper!C11=0, "", upper!C11)</f>
+        <f>IF(upper!C11="", "", upper!C11)</f>
         <v/>
       </c>
       <c r="D80" s="72" t="str">
-        <f>IF(upper!D11=0, "", upper!D11)</f>
+        <f>IF(upper!D11="", "", upper!D11)</f>
         <v/>
       </c>
       <c r="E80" s="72" t="str">
-        <f>IF(upper!E11=0, "", upper!E11)</f>
-        <v/>
-      </c>
-      <c r="F80" s="64" t="str">
-        <f>IF(upper!F11=0, "", upper!F11)</f>
-        <v/>
-      </c>
-      <c r="G80" s="64" t="str">
-        <f>IF(upper!A11=0, "", upper!G11)</f>
+        <f>IF(upper!E11="", "", upper!E11)</f>
+        <v/>
+      </c>
+      <c r="F80" s="72" t="str">
+        <f>IF(upper!F11="", "", upper!F11)</f>
+        <v/>
+      </c>
+      <c r="G80" s="72" t="str">
+        <f>IF(upper!G11="", "", upper!G11)</f>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="64" t="str">
-        <f>IF(upper!A12=0, "", upper!A12)</f>
+        <f>IF(upper!A12="", "", upper!A12)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B81" s="64">
-        <f>IF(upper!B12=0, "", upper!B12)</f>
+      <c r="B81" s="72">
+        <f>IF(upper!B12="", "", upper!B12)</f>
         <v>61</v>
       </c>
       <c r="C81" s="72">
-        <f>IF(upper!C12=0, "", upper!C12)</f>
+        <f>IF(upper!C12="", "", upper!C12)</f>
         <v>22</v>
       </c>
       <c r="D81" s="72">
-        <f>IF(upper!D12=0, "", upper!D12)</f>
+        <f>IF(upper!D12="", "", upper!D12)</f>
         <v>236.95041722813599</v>
       </c>
       <c r="E81" s="72">
-        <f>IF(upper!E12=0, "", upper!E12)</f>
+        <f>IF(upper!E12="", "", upper!E12)</f>
         <v>-59.999859694228427</v>
       </c>
-      <c r="F81" s="64">
-        <f>IF(upper!F12=0, "", upper!F12)</f>
+      <c r="F81" s="72">
+        <f>IF(upper!F12="", "", upper!F12)</f>
         <v>5</v>
       </c>
-      <c r="G81" s="64">
-        <f>IF(upper!A12=0, "", upper!G12)</f>
+      <c r="G81" s="72">
+        <f>IF(upper!G12="", "", upper!G12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="64" t="str">
-        <f>IF(upper!A13=0, "", upper!A13)</f>
+        <f>IF(upper!A13="", "", upper!A13)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B82" s="64">
-        <f>IF(upper!B13=0, "", upper!B13)</f>
+      <c r="B82" s="72">
+        <f>IF(upper!B13="", "", upper!B13)</f>
         <v>56</v>
       </c>
       <c r="C82" s="72">
-        <f>IF(upper!C13=0, "", upper!C13)</f>
+        <f>IF(upper!C13="", "", upper!C13)</f>
         <v>22</v>
       </c>
       <c r="D82" s="72">
-        <f>IF(upper!D13=0, "", upper!D13)</f>
+        <f>IF(upper!D13="", "", upper!D13)</f>
         <v>255.425625842204</v>
       </c>
-      <c r="E82" s="72" t="str">
-        <f>IF(upper!E13=0, "", upper!E13)</f>
-        <v/>
-      </c>
-      <c r="F82" s="64">
-        <f>IF(upper!F13=0, "", upper!F13)</f>
+      <c r="E82" s="72">
+        <f>IF(upper!E13="", "", upper!E13)</f>
+        <v>0</v>
+      </c>
+      <c r="F82" s="72">
+        <f>IF(upper!F13="", "", upper!F13)</f>
         <v>5</v>
       </c>
-      <c r="G82" s="64">
-        <f>IF(upper!A13=0, "", upper!G13)</f>
+      <c r="G82" s="72">
+        <f>IF(upper!G13="", "", upper!G13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="64" t="str">
-        <f>IF(upper!A14=0, "", upper!A14)</f>
+        <f>IF(upper!A14="", "", upper!A14)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B83" s="64">
-        <f>IF(upper!B14=0, "", upper!B14)</f>
+      <c r="B83" s="72">
+        <f>IF(upper!B14="", "", upper!B14)</f>
         <v>57</v>
       </c>
       <c r="C83" s="72">
-        <f>IF(upper!C14=0, "", upper!C14)</f>
+        <f>IF(upper!C14="", "", upper!C14)</f>
         <v>6</v>
       </c>
       <c r="D83" s="72">
-        <f>IF(upper!D14=0, "", upper!D14)</f>
+        <f>IF(upper!D14="", "", upper!D14)</f>
         <v>264.66323014923796</v>
       </c>
       <c r="E83" s="72">
-        <f>IF(upper!E14=0, "", upper!E14)</f>
+        <f>IF(upper!E14="", "", upper!E14)</f>
         <v>59.999859694228427</v>
       </c>
-      <c r="F83" s="64">
-        <f>IF(upper!F14=0, "", upper!F14)</f>
+      <c r="F83" s="72">
+        <f>IF(upper!F14="", "", upper!F14)</f>
         <v>5</v>
       </c>
-      <c r="G83" s="64">
-        <f>IF(upper!A14=0, "", upper!G14)</f>
+      <c r="G83" s="72">
+        <f>IF(upper!G14="", "", upper!G14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="64" t="str">
-        <f>IF(upper!A15=0, "", upper!A15)</f>
-        <v/>
-      </c>
-      <c r="B84" s="64" t="str">
-        <f>IF(upper!B15=0, "", upper!B15)</f>
+        <f>IF(upper!A15="", "", upper!A15)</f>
+        <v/>
+      </c>
+      <c r="B84" s="72" t="str">
+        <f>IF(upper!B15="", "", upper!B15)</f>
         <v/>
       </c>
       <c r="C84" s="72" t="str">
-        <f>IF(upper!C15=0, "", upper!C15)</f>
+        <f>IF(upper!C15="", "", upper!C15)</f>
         <v/>
       </c>
       <c r="D84" s="72" t="str">
-        <f>IF(upper!D15=0, "", upper!D15)</f>
+        <f>IF(upper!D15="", "", upper!D15)</f>
         <v/>
       </c>
       <c r="E84" s="72" t="str">
-        <f>IF(upper!E15=0, "", upper!E15)</f>
-        <v/>
-      </c>
-      <c r="F84" s="64" t="str">
-        <f>IF(upper!F15=0, "", upper!F15)</f>
-        <v/>
-      </c>
-      <c r="G84" s="64" t="str">
-        <f>IF(upper!A15=0, "", upper!G15)</f>
+        <f>IF(upper!E15="", "", upper!E15)</f>
+        <v/>
+      </c>
+      <c r="F84" s="72" t="str">
+        <f>IF(upper!F15="", "", upper!F15)</f>
+        <v/>
+      </c>
+      <c r="G84" s="72" t="str">
+        <f>IF(upper!G15="", "", upper!G15)</f>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="64" t="str">
-        <f>IF(upper!A16=0, "", upper!A16)</f>
-        <v/>
-      </c>
-      <c r="B85" s="64" t="str">
-        <f>IF(upper!B16=0, "", upper!B16)</f>
+        <f>IF(upper!A16="", "", upper!A16)</f>
+        <v/>
+      </c>
+      <c r="B85" s="72" t="str">
+        <f>IF(upper!B16="", "", upper!B16)</f>
         <v/>
       </c>
       <c r="C85" s="72" t="str">
-        <f>IF(upper!C16=0, "", upper!C16)</f>
+        <f>IF(upper!C16="", "", upper!C16)</f>
         <v/>
       </c>
       <c r="D85" s="72" t="str">
-        <f>IF(upper!D16=0, "", upper!D16)</f>
+        <f>IF(upper!D16="", "", upper!D16)</f>
         <v/>
       </c>
       <c r="E85" s="72" t="str">
-        <f>IF(upper!E16=0, "", upper!E16)</f>
-        <v/>
-      </c>
-      <c r="F85" s="64" t="str">
-        <f>IF(upper!F16=0, "", upper!F16)</f>
-        <v/>
-      </c>
-      <c r="G85" s="64" t="str">
-        <f>IF(upper!A16=0, "", upper!G16)</f>
+        <f>IF(upper!E16="", "", upper!E16)</f>
+        <v/>
+      </c>
+      <c r="F85" s="72" t="str">
+        <f>IF(upper!F16="", "", upper!F16)</f>
+        <v/>
+      </c>
+      <c r="G85" s="72" t="str">
+        <f>IF(upper!G16="", "", upper!G16)</f>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="str">
-        <f>IF(upper!A17=0, "", upper!A17)</f>
-        <v/>
-      </c>
-      <c r="B86" s="64" t="str">
-        <f>IF(upper!B17=0, "", upper!B17)</f>
+        <f>IF(upper!A17="", "", upper!A17)</f>
+        <v/>
+      </c>
+      <c r="B86" s="72" t="str">
+        <f>IF(upper!B17="", "", upper!B17)</f>
         <v/>
       </c>
       <c r="C86" s="72" t="str">
-        <f>IF(upper!C17=0, "", upper!C17)</f>
+        <f>IF(upper!C17="", "", upper!C17)</f>
         <v/>
       </c>
       <c r="D86" s="72" t="str">
-        <f>IF(upper!D17=0, "", upper!D17)</f>
+        <f>IF(upper!D17="", "", upper!D17)</f>
         <v/>
       </c>
       <c r="E86" s="72" t="str">
-        <f>IF(upper!E17=0, "", upper!E17)</f>
-        <v/>
-      </c>
-      <c r="F86" s="64" t="str">
-        <f>IF(upper!F17=0, "", upper!F17)</f>
-        <v/>
-      </c>
-      <c r="G86" s="64" t="str">
-        <f>IF(upper!A17=0, "", upper!G17)</f>
+        <f>IF(upper!E17="", "", upper!E17)</f>
+        <v/>
+      </c>
+      <c r="F86" s="72" t="str">
+        <f>IF(upper!F17="", "", upper!F17)</f>
+        <v/>
+      </c>
+      <c r="G86" s="72" t="str">
+        <f>IF(upper!G17="", "", upper!G17)</f>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="str">
-        <f>IF(upper!A18=0, "", upper!A18)</f>
-        <v/>
-      </c>
-      <c r="B87" s="64" t="str">
-        <f>IF(upper!B18=0, "", upper!B18)</f>
+        <f>IF(upper!A18="", "", upper!A18)</f>
+        <v/>
+      </c>
+      <c r="B87" s="72" t="str">
+        <f>IF(upper!B18="", "", upper!B18)</f>
         <v/>
       </c>
       <c r="C87" s="72" t="str">
-        <f>IF(upper!C18=0, "", upper!C18)</f>
+        <f>IF(upper!C18="", "", upper!C18)</f>
         <v/>
       </c>
       <c r="D87" s="72" t="str">
-        <f>IF(upper!D18=0, "", upper!D18)</f>
+        <f>IF(upper!D18="", "", upper!D18)</f>
         <v/>
       </c>
       <c r="E87" s="72" t="str">
-        <f>IF(upper!E18=0, "", upper!E18)</f>
-        <v/>
-      </c>
-      <c r="F87" s="64" t="str">
-        <f>IF(upper!F18=0, "", upper!F18)</f>
-        <v/>
-      </c>
-      <c r="G87" s="64" t="str">
-        <f>IF(upper!A18=0, "", upper!G18)</f>
+        <f>IF(upper!E18="", "", upper!E18)</f>
+        <v/>
+      </c>
+      <c r="F87" s="72" t="str">
+        <f>IF(upper!F18="", "", upper!F18)</f>
+        <v/>
+      </c>
+      <c r="G87" s="72" t="str">
+        <f>IF(upper!G18="", "", upper!G18)</f>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="str">
-        <f>IF(upper!A19=0, "", upper!A19)</f>
+        <f>IF(upper!A19="", "", upper!A19)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B88" s="64">
-        <f>IF(upper!B19=0, "", upper!B19)</f>
+      <c r="B88" s="72">
+        <f>IF(upper!B19="", "", upper!B19)</f>
         <v>58</v>
       </c>
       <c r="C88" s="72">
-        <f>IF(upper!C19=0, "", upper!C19)</f>
+        <f>IF(upper!C19="", "", upper!C19)</f>
         <v>-10</v>
       </c>
       <c r="D88" s="72">
-        <f>IF(upper!D19=0, "", upper!D19)</f>
+        <f>IF(upper!D19="", "", upper!D19)</f>
         <v>255.425625842204</v>
       </c>
       <c r="E88" s="72">
-        <f>IF(upper!E19=0, "", upper!E19)</f>
+        <f>IF(upper!E19="", "", upper!E19)</f>
         <v>119.99971938845685</v>
       </c>
-      <c r="F88" s="64">
-        <f>IF(upper!F19=0, "", upper!F19)</f>
+      <c r="F88" s="72">
+        <f>IF(upper!F19="", "", upper!F19)</f>
         <v>5</v>
       </c>
-      <c r="G88" s="64">
-        <f>IF(upper!A19=0, "", upper!G19)</f>
+      <c r="G88" s="72">
+        <f>IF(upper!G19="", "", upper!G19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="64" t="str">
-        <f>IF(upper!A20=0, "", upper!A20)</f>
+        <f>IF(upper!A20="", "", upper!A20)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B89" s="64">
-        <f>IF(upper!B20=0, "", upper!B20)</f>
+      <c r="B89" s="72">
+        <f>IF(upper!B20="", "", upper!B20)</f>
         <v>53</v>
       </c>
       <c r="C89" s="72">
-        <f>IF(upper!C20=0, "", upper!C20)</f>
+        <f>IF(upper!C20="", "", upper!C20)</f>
         <v>-26</v>
       </c>
       <c r="D89" s="72">
-        <f>IF(upper!D20=0, "", upper!D20)</f>
+        <f>IF(upper!D20="", "", upper!D20)</f>
         <v>264.66323014923796</v>
       </c>
       <c r="E89" s="72">
-        <f>IF(upper!E20=0, "", upper!E20)</f>
+        <f>IF(upper!E20="", "", upper!E20)</f>
         <v>59.999859694228427</v>
       </c>
-      <c r="F89" s="64">
-        <f>IF(upper!F20=0, "", upper!F20)</f>
+      <c r="F89" s="72">
+        <f>IF(upper!F20="", "", upper!F20)</f>
         <v>5</v>
       </c>
-      <c r="G89" s="64">
-        <f>IF(upper!A20=0, "", upper!G20)</f>
+      <c r="G89" s="72">
+        <f>IF(upper!G20="", "", upper!G20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="64" t="str">
-        <f>IF(upper!A21=0, "", upper!A21)</f>
+        <f>IF(upper!A21="", "", upper!A21)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B90" s="64">
-        <f>IF(upper!B21=0, "", upper!B21)</f>
+      <c r="B90" s="72">
+        <f>IF(upper!B21="", "", upper!B21)</f>
         <v>63</v>
       </c>
       <c r="C90" s="72">
-        <f>IF(upper!C21=0, "", upper!C21)</f>
+        <f>IF(upper!C21="", "", upper!C21)</f>
         <v>-42</v>
       </c>
       <c r="D90" s="72">
-        <f>IF(upper!D21=0, "", upper!D21)</f>
+        <f>IF(upper!D21="", "", upper!D21)</f>
         <v>255.425625842204</v>
       </c>
       <c r="E90" s="72">
-        <f>IF(upper!E21=0, "", upper!E21)</f>
+        <f>IF(upper!E21="", "", upper!E21)</f>
         <v>119.99971938845685</v>
       </c>
-      <c r="F90" s="64">
-        <f>IF(upper!F21=0, "", upper!F21)</f>
+      <c r="F90" s="72">
+        <f>IF(upper!F21="", "", upper!F21)</f>
         <v>5</v>
       </c>
-      <c r="G90" s="64">
-        <f>IF(upper!A21=0, "", upper!G21)</f>
+      <c r="G90" s="72">
+        <f>IF(upper!G21="", "", upper!G21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="64" t="str">
-        <f>IF(upper!A22=0, "", upper!A22)</f>
+        <f>IF(upper!A22="", "", upper!A22)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B91" s="64">
-        <f>IF(upper!B22=0, "", upper!B22)</f>
+      <c r="B91" s="72">
+        <f>IF(upper!B22="", "", upper!B22)</f>
         <v>48</v>
       </c>
       <c r="C91" s="72">
-        <f>IF(upper!C22=0, "", upper!C22)</f>
+        <f>IF(upper!C22="", "", upper!C22)</f>
         <v>-42</v>
       </c>
       <c r="D91" s="72">
-        <f>IF(upper!D22=0, "", upper!D22)</f>
+        <f>IF(upper!D22="", "", upper!D22)</f>
         <v>236.95041722813599</v>
       </c>
       <c r="E91" s="72">
-        <f>IF(upper!E22=0, "", upper!E22)</f>
+        <f>IF(upper!E22="", "", upper!E22)</f>
         <v>179.99957908268468</v>
       </c>
-      <c r="F91" s="64">
-        <f>IF(upper!F22=0, "", upper!F22)</f>
+      <c r="F91" s="72">
+        <f>IF(upper!F22="", "", upper!F22)</f>
         <v>5</v>
       </c>
-      <c r="G91" s="64">
-        <f>IF(upper!A22=0, "", upper!G22)</f>
+      <c r="G91" s="72">
+        <f>IF(upper!G22="", "", upper!G22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="64" t="str">
-        <f>IF(upper!A23=0, "", upper!A23)</f>
+        <f>IF(upper!A23="", "", upper!A23)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B92" s="64">
-        <f>IF(upper!B23=0, "", upper!B23)</f>
+      <c r="B92" s="72">
+        <f>IF(upper!B23="", "", upper!B23)</f>
         <v>59</v>
       </c>
       <c r="C92" s="72">
-        <f>IF(upper!C23=0, "", upper!C23)</f>
+        <f>IF(upper!C23="", "", upper!C23)</f>
         <v>-10</v>
       </c>
       <c r="D92" s="72">
-        <f>IF(upper!D23=0, "", upper!D23)</f>
+        <f>IF(upper!D23="", "", upper!D23)</f>
         <v>236.95041722813599</v>
       </c>
       <c r="E92" s="72">
-        <f>IF(upper!E23=0, "", upper!E23)</f>
+        <f>IF(upper!E23="", "", upper!E23)</f>
         <v>179.99957908268468</v>
       </c>
-      <c r="F92" s="64">
-        <f>IF(upper!F23=0, "", upper!F23)</f>
+      <c r="F92" s="72">
+        <f>IF(upper!F23="", "", upper!F23)</f>
         <v>5</v>
       </c>
-      <c r="G92" s="64">
-        <f>IF(upper!A23=0, "", upper!G23)</f>
+      <c r="G92" s="72">
+        <f>IF(upper!G23="", "", upper!G23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="64" t="str">
-        <f>IF(upper!A24=0, "", upper!A24)</f>
-        <v/>
-      </c>
-      <c r="B93" s="64" t="str">
-        <f>IF(upper!B24=0, "", upper!B24)</f>
+        <f>IF(upper!A24="", "", upper!A24)</f>
+        <v/>
+      </c>
+      <c r="B93" s="72" t="str">
+        <f>IF(upper!B24="", "", upper!B24)</f>
         <v/>
       </c>
       <c r="C93" s="72" t="str">
-        <f>IF(upper!C24=0, "", upper!C24)</f>
+        <f>IF(upper!C24="", "", upper!C24)</f>
         <v/>
       </c>
       <c r="D93" s="72" t="str">
-        <f>IF(upper!D24=0, "", upper!D24)</f>
+        <f>IF(upper!D24="", "", upper!D24)</f>
         <v/>
       </c>
       <c r="E93" s="72" t="str">
-        <f>IF(upper!E24=0, "", upper!E24)</f>
-        <v/>
-      </c>
-      <c r="F93" s="64" t="str">
-        <f>IF(upper!F24=0, "", upper!F24)</f>
-        <v/>
-      </c>
-      <c r="G93" s="64" t="str">
-        <f>IF(upper!A24=0, "", upper!G24)</f>
+        <f>IF(upper!E24="", "", upper!E24)</f>
+        <v/>
+      </c>
+      <c r="F93" s="72" t="str">
+        <f>IF(upper!F24="", "", upper!F24)</f>
+        <v/>
+      </c>
+      <c r="G93" s="72" t="str">
+        <f>IF(upper!G24="", "", upper!G24)</f>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="64" t="str">
-        <f>IF(upper!A25=0, "", upper!A25)</f>
-        <v/>
-      </c>
-      <c r="B94" s="64" t="str">
-        <f>IF(upper!B25=0, "", upper!B25)</f>
+        <f>IF(upper!A25="", "", upper!A25)</f>
+        <v/>
+      </c>
+      <c r="B94" s="72" t="str">
+        <f>IF(upper!B25="", "", upper!B25)</f>
         <v/>
       </c>
       <c r="C94" s="72" t="str">
-        <f>IF(upper!C25=0, "", upper!C25)</f>
+        <f>IF(upper!C25="", "", upper!C25)</f>
         <v/>
       </c>
       <c r="D94" s="72" t="str">
-        <f>IF(upper!D25=0, "", upper!D25)</f>
+        <f>IF(upper!D25="", "", upper!D25)</f>
         <v/>
       </c>
       <c r="E94" s="72" t="str">
-        <f>IF(upper!E25=0, "", upper!E25)</f>
-        <v/>
-      </c>
-      <c r="F94" s="64" t="str">
-        <f>IF(upper!F25=0, "", upper!F25)</f>
-        <v/>
-      </c>
-      <c r="G94" s="64" t="str">
-        <f>IF(upper!A25=0, "", upper!G25)</f>
+        <f>IF(upper!E25="", "", upper!E25)</f>
+        <v/>
+      </c>
+      <c r="F94" s="72" t="str">
+        <f>IF(upper!F25="", "", upper!F25)</f>
+        <v/>
+      </c>
+      <c r="G94" s="72" t="str">
+        <f>IF(upper!G25="", "", upper!G25)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
added info about triangles connected
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/leftArm_ini_generator new.xlsx
+++ b/app/skinGui/iniGenerators/leftArm_ini_generator new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="-15" windowWidth="13590" windowHeight="10110"/>
+    <workbookView xWindow="5055" yWindow="-15" windowWidth="13590" windowHeight="10110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="lower" sheetId="1" r:id="rId1"/>
@@ -12135,8 +12135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13106,7 +13106,7 @@
       <c r="L23" s="5">
         <v>33</v>
       </c>
-      <c r="M23" s="76">
+      <c r="M23" s="75">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -13139,7 +13139,7 @@
       <c r="L24" s="5">
         <v>42</v>
       </c>
-      <c r="M24" s="75">
+      <c r="M24" s="76">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -13475,8 +13475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13592,7 +13592,7 @@
       <c r="L3" s="13">
         <v>10</v>
       </c>
-      <c r="M3" s="76">
+      <c r="M3" s="75">
         <f>(ROUND((L3/10),0)-1)*4+(MOD(L3,10))</f>
         <v>0</v>
       </c>
@@ -13657,7 +13657,7 @@
       <c r="L4" s="5">
         <v>11</v>
       </c>
-      <c r="M4" s="76">
+      <c r="M4" s="75">
         <f t="shared" ref="M4:M25" si="5">(ROUND((L4/10),0)-1)*4+(MOD(L4,10))</f>
         <v>1</v>
       </c>
@@ -14675,7 +14675,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14790,7 +14790,7 @@
       <c r="L3" s="13">
         <v>10</v>
       </c>
-      <c r="M3" s="76">
+      <c r="M3" s="75">
         <f>(ROUND((L3/10),0)-1)*4+(MOD(L3,10))</f>
         <v>0</v>
       </c>
@@ -14855,7 +14855,7 @@
       <c r="L4" s="5">
         <v>11</v>
       </c>
-      <c r="M4" s="76">
+      <c r="M4" s="75">
         <f t="shared" ref="M4:M25" si="5">(ROUND((L4/10),0)-1)*4+(MOD(L4,10))</f>
         <v>1</v>
       </c>
@@ -14917,7 +14917,7 @@
       <c r="L5" s="5">
         <v>12</v>
       </c>
-      <c r="M5" s="76">
+      <c r="M5" s="75">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
@@ -14978,7 +14978,7 @@
       <c r="L6" s="5">
         <v>13</v>
       </c>
-      <c r="M6" s="76">
+      <c r="M6" s="75">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
@@ -15037,7 +15037,7 @@
       <c r="L7" s="5">
         <v>20</v>
       </c>
-      <c r="M7" s="76">
+      <c r="M7" s="75">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
@@ -15095,7 +15095,7 @@
       <c r="L8" s="5">
         <v>21</v>
       </c>
-      <c r="M8" s="76">
+      <c r="M8" s="75">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
@@ -15152,7 +15152,7 @@
       <c r="L9" s="5">
         <v>22</v>
       </c>
-      <c r="M9" s="76">
+      <c r="M9" s="75">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
@@ -15207,7 +15207,7 @@
       <c r="L10" s="5">
         <v>23</v>
       </c>
-      <c r="M10" s="76">
+      <c r="M10" s="75">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
@@ -15261,7 +15261,7 @@
       <c r="L11" s="5">
         <v>40</v>
       </c>
-      <c r="M11" s="76">
+      <c r="M11" s="75">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
@@ -15316,7 +15316,7 @@
       <c r="L12" s="5">
         <v>41</v>
       </c>
-      <c r="M12" s="76">
+      <c r="M12" s="75">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
@@ -15368,7 +15368,7 @@
       <c r="L13" s="5">
         <v>30</v>
       </c>
-      <c r="M13" s="76">
+      <c r="M13" s="75">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
@@ -15861,7 +15861,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15869,8 +15870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16339,7 +16340,7 @@
       <c r="L12" s="5">
         <v>41</v>
       </c>
-      <c r="M12" s="76">
+      <c r="M12" s="75">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -16391,7 +16392,7 @@
       <c r="L13" s="5">
         <v>30</v>
       </c>
-      <c r="M13" s="76">
+      <c r="M13" s="75">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -16443,7 +16444,7 @@
       <c r="L14" s="5">
         <v>31</v>
       </c>
-      <c r="M14" s="76">
+      <c r="M14" s="75">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -16627,7 +16628,7 @@
       <c r="L19" s="5">
         <v>32</v>
       </c>
-      <c r="M19" s="76">
+      <c r="M19" s="75">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -16679,7 +16680,7 @@
       <c r="L20" s="5">
         <v>21</v>
       </c>
-      <c r="M20" s="76">
+      <c r="M20" s="75">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -16731,7 +16732,7 @@
       <c r="L21" s="5">
         <v>43</v>
       </c>
-      <c r="M21" s="76">
+      <c r="M21" s="75">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -16783,7 +16784,7 @@
       <c r="L22" s="5">
         <v>10</v>
       </c>
-      <c r="M22" s="76">
+      <c r="M22" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -16835,7 +16836,7 @@
       <c r="L23" s="5">
         <v>33</v>
       </c>
-      <c r="M23" s="76">
+      <c r="M23" s="75">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>

</xml_diff>